<commit_message>
action list updated and project description downloaded
</commit_message>
<xml_diff>
--- a/Reports/Action List.xlsx
+++ b/Reports/Action List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Home Page" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="Profile Page 1" sheetId="1" r:id="rId4"/>
     <sheet name="Profile Page 2" sheetId="5" r:id="rId5"/>
     <sheet name="Reports" sheetId="6" r:id="rId6"/>
+    <sheet name="Testing Requirements" sheetId="7" r:id="rId7"/>
+    <sheet name="DatesGrade Structure" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="106">
   <si>
     <t xml:space="preserve">lot of informaiton -  </t>
   </si>
@@ -200,13 +202,172 @@
   </si>
   <si>
     <t>Weekly Update w/e 03 Aug</t>
+  </si>
+  <si>
+    <t>30 User profiles Set up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Organizations </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open </t>
+  </si>
+  <si>
+    <t>Need to understand what is needed</t>
+  </si>
+  <si>
+    <t>Final Project Report</t>
+  </si>
+  <si>
+    <t>1   </t>
+  </si>
+  <si>
+    <t>July 23rd</t>
+  </si>
+  <si>
+    <t>Work on website</t>
+  </si>
+  <si>
+    <t>12   </t>
+  </si>
+  <si>
+    <t>July 30th</t>
+  </si>
+  <si>
+    <r>
+      <t>Final product due </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>August 5th</t>
+    </r>
+  </si>
+  <si>
+    <t>Grading Structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Design document (Sunday, June 24th): 20%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database implementation (Sunday, July 1st): 5% </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prototype (Sunday, July 15th): 5% </t>
+  </si>
+  <si>
+    <t>Software Test Report (Sunday, July 22nd) 5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Implementation (Sunday, August 5th): 40%</t>
+  </si>
+  <si>
+    <t>Documentation: 5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mid term exam (May 30th): 20% </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Three staff members will test the functionality described in the Project </t>
+  </si>
+  <si>
+    <t>Three staff members will test the functionality described in the Project Overview, this will include:</t>
+  </si>
+  <si>
+    <t>Registering as users and creating profiles;</t>
+  </si>
+  <si>
+    <t>Browsing users (without specific search terms);</t>
+  </si>
+  <si>
+    <t>Searching for users (including each other);</t>
+  </si>
+  <si>
+    <t>Observing the automatic suggestions;</t>
+  </si>
+  <si>
+    <t>Connecting to each other</t>
+  </si>
+  <si>
+    <t>Logging in as site administrator (your final report will need to describe how to do this, see below)</t>
+  </si>
+  <si>
+    <t>The demo will be conducted using two different web browsers (we recommend Firefox and Google Chrome, but the group can decide);</t>
+  </si>
+  <si>
+    <t>A final report using the headings described below needs to be uploaded to Moodle by August 5th</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>High level functionality</t>
+  </si>
+  <si>
+    <t>Web page mock ups</t>
+  </si>
+  <si>
+    <t>Database tables</t>
+  </si>
+  <si>
+    <t>User testing (how you reacted to the user tests from deliverable 5)</t>
+  </si>
+  <si>
+    <t>Extras (any extra functionality that you added over the initial brief)</t>
+  </si>
+  <si>
+    <t>Administration detail (how can we log on as administrator to your site)</t>
+  </si>
+  <si>
+    <t>Sources (list any items such as images that you took from somewhere, showing the image and the original source)</t>
+  </si>
+  <si>
+    <t>In particular, note any deviations from the original design</t>
+  </si>
+  <si>
+    <t>additonal thoughts based on the testing exercise</t>
+  </si>
+  <si>
+    <t>1. Was there an index.html file? Was it obvious what the website was from the first page?</t>
+  </si>
+  <si>
+    <t>1. What is the site for? Describe the industry that the site targets.</t>
+  </si>
+  <si>
+    <t>1. How well did the individual registration section work? What happened when you put in malformed input (for example, mismatched passwords, wrong types, etc.)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Did the search function work? </t>
+  </si>
+  <si>
+    <t>1. What was the “look and feel” of the site like? Was it pleasant to use or were there rendering problems and/or missing links?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>need to update current mockups</t>
+  </si>
+  <si>
+    <t>take from original and update</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>Update if needed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,16 +375,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -231,12 +417,126 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFE8E8E8"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFE8E8E8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFE8E8E8"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFE8E8E8"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFE8E8E8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFE8E8E8"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFE8E8E8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFE8E8E8"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFE8E8E8"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFE8E8E8"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFE8E8E8"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFE8E8E8"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFE8E8E8"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFE8E8E8"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -984,18 +1284,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:D5"/>
+  <dimension ref="C4:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="31.42578125" customWidth="1"/>
+    <col min="3" max="3" width="108.140625" customWidth="1"/>
+    <col min="5" max="5" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>55</v>
       </c>
@@ -1003,15 +1304,356 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>56</v>
       </c>
       <c r="D5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="110.140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="54.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="48" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="77.25" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
udpates to Action list
</commit_message>
<xml_diff>
--- a/Reports/Action List.xlsx
+++ b/Reports/Action List.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Home Page" sheetId="2" r:id="rId1"/>
-    <sheet name="Register" sheetId="3" r:id="rId2"/>
-    <sheet name="meeting space" sheetId="4" r:id="rId3"/>
-    <sheet name="Profile Page 1" sheetId="1" r:id="rId4"/>
-    <sheet name="Profile Page 2" sheetId="5" r:id="rId5"/>
-    <sheet name="Reports" sheetId="6" r:id="rId6"/>
-    <sheet name="Testing Requirements" sheetId="7" r:id="rId7"/>
-    <sheet name="DatesGrade Structure" sheetId="8" r:id="rId8"/>
+    <sheet name="Logon" sheetId="9" r:id="rId2"/>
+    <sheet name="Register" sheetId="3" r:id="rId3"/>
+    <sheet name="meeting space" sheetId="4" r:id="rId4"/>
+    <sheet name="Profile Page 1" sheetId="1" r:id="rId5"/>
+    <sheet name="Profile Page 2" sheetId="5" r:id="rId6"/>
+    <sheet name="Reports" sheetId="6" r:id="rId7"/>
+    <sheet name="Testing Requirements" sheetId="7" r:id="rId8"/>
+    <sheet name="DatesGrade Structure" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="124">
   <si>
     <t xml:space="preserve">lot of informaiton -  </t>
   </si>
@@ -361,6 +362,60 @@
   </si>
   <si>
     <t>Update if needed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menu not working </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forgot Password Option </t>
+  </si>
+  <si>
+    <t>Allowed me to enter email but did not receive email</t>
+  </si>
+  <si>
+    <t>Basic functionality of this Page only</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Logon  Type email Deirdre.Shanahan@gmail.com</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>Test2</t>
+  </si>
+  <si>
+    <t>Option</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Logon as Lisa Sharp Password welcomE01#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allowed me to logon and took me to Meeting Space </t>
+  </si>
+  <si>
+    <t>Welcome Lisa at the top of meeting space</t>
+  </si>
+  <si>
+    <t>looks good so far</t>
+  </si>
+  <si>
+    <t>Test 3</t>
+  </si>
+  <si>
+    <t>Logon as  Carol.James@gmail.com password welcomE01#</t>
+  </si>
+  <si>
+    <t>Logon opttion</t>
+  </si>
+  <si>
+    <t>Brought me to meeting space but error because of Profile Screen 2</t>
   </si>
 </sst>
 </file>
@@ -395,7 +450,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -405,6 +460,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -511,7 +572,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -537,6 +598,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -817,10 +879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E4"/>
+  <dimension ref="B1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,12 +932,116 @@
         <v>8</v>
       </c>
     </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="50.5703125" customWidth="1"/>
+    <col min="4" max="4" width="41" customWidth="1"/>
+    <col min="5" max="5" width="40" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D5"/>
   <sheetViews>
@@ -935,12 +1101,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C9"/>
+  <dimension ref="B2:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,12 +1172,20 @@
         <v>21</v>
       </c>
     </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:E20"/>
   <sheetViews>
@@ -1268,7 +1442,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1282,11 +1456,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -1409,7 +1583,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D22"/>
   <sheetViews>
@@ -1573,7 +1747,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E13"/>
   <sheetViews>
@@ -1586,7 +1760,7 @@
     <col min="5" max="5" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
updated with new tests
</commit_message>
<xml_diff>
--- a/Reports/Action List.xlsx
+++ b/Reports/Action List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Home Page" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="145">
   <si>
     <t xml:space="preserve">lot of informaiton -  </t>
   </si>
@@ -421,9 +421,6 @@
     <t>Logon option</t>
   </si>
   <si>
-    <t xml:space="preserve">First screen works, second screen display but </t>
-  </si>
-  <si>
     <t>logon as Lisa Sharp</t>
   </si>
   <si>
@@ -450,6 +447,42 @@
   </si>
   <si>
     <t>Test 6</t>
+  </si>
+  <si>
+    <t>First screen works, second screen display but save not functioning</t>
+  </si>
+  <si>
+    <t>Test 7</t>
+  </si>
+  <si>
+    <t>logon/Meeting Space</t>
+  </si>
+  <si>
+    <t>chatting with Paul even though she wants Female ?</t>
+  </si>
+  <si>
+    <t>Bad Data in Data base</t>
+  </si>
+  <si>
+    <t>Test 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You are chatting with  No Mathces Found </t>
+  </si>
+  <si>
+    <t>Need clarify on message</t>
+  </si>
+  <si>
+    <t>Test 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matched with Male when she wants a female </t>
+  </si>
+  <si>
+    <t>Logon as Jacob.Newman@gmail.com Password welcomeE01</t>
+  </si>
+  <si>
+    <t>none of the buttons in system  functional yet</t>
   </si>
 </sst>
 </file>
@@ -978,20 +1011,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F13"/>
+  <dimension ref="B1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="50.5703125" customWidth="1"/>
     <col min="4" max="4" width="41" customWidth="1"/>
-    <col min="5" max="5" width="40" style="7" customWidth="1"/>
+    <col min="5" max="5" width="50.5703125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>113</v>
       </c>
@@ -1002,7 +1036,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>111</v>
       </c>
@@ -1019,7 +1053,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>101</v>
       </c>
@@ -1033,7 +1067,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>112</v>
       </c>
@@ -1046,13 +1080,19 @@
       <c r="E6" s="7" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>120</v>
       </c>
@@ -1066,10 +1106,10 @@
         <v>122</v>
       </c>
       <c r="F9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>123</v>
       </c>
@@ -1077,46 +1117,120 @@
         <v>121</v>
       </c>
       <c r="D11" t="s">
+        <v>127</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" t="s">
         <v>128</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E12" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" t="s">
         <v>125</v>
       </c>
-      <c r="F11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>127</v>
-      </c>
-      <c r="C12" t="s">
-        <v>126</v>
-      </c>
-      <c r="D12" t="s">
-        <v>129</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="F12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="165" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>133</v>
-      </c>
-      <c r="C13" t="s">
-        <v>132</v>
-      </c>
-      <c r="D13" t="s">
-        <v>129</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="D14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D15" t="s">
+        <v>135</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C16" t="s">
+        <v>121</v>
+      </c>
+      <c r="D16" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="F16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>143</v>
+      </c>
+      <c r="D17" t="s">
+        <v>135</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="F17" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1274,7 +1388,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -1546,17 +1660,17 @@
   <dimension ref="C4:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="108.140625" customWidth="1"/>
+    <col min="3" max="3" width="83" style="7" customWidth="1"/>
     <col min="5" max="5" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+      <c r="C4" s="7" t="s">
         <v>55</v>
       </c>
       <c r="D4" t="s">
@@ -1564,7 +1678,7 @@
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+      <c r="C5" s="7" t="s">
         <v>56</v>
       </c>
       <c r="D5" t="s">
@@ -1572,7 +1686,7 @@
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+      <c r="C7" s="7" t="s">
         <v>61</v>
       </c>
       <c r="D7" t="s">
@@ -1580,7 +1694,7 @@
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+      <c r="C8" s="7" t="s">
         <v>86</v>
       </c>
       <c r="D8" t="s">
@@ -1591,7 +1705,7 @@
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+      <c r="C9" s="7" t="s">
         <v>87</v>
       </c>
       <c r="D9" t="s">
@@ -1602,7 +1716,7 @@
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+      <c r="C10" s="7" t="s">
         <v>88</v>
       </c>
       <c r="D10" t="s">
@@ -1613,7 +1727,7 @@
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+      <c r="C11" s="7" t="s">
         <v>89</v>
       </c>
       <c r="D11" t="s">
@@ -1624,7 +1738,7 @@
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+      <c r="C12" s="7" t="s">
         <v>90</v>
       </c>
       <c r="D12" t="s">
@@ -1632,7 +1746,7 @@
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+      <c r="C13" s="7" t="s">
         <v>91</v>
       </c>
       <c r="D13" t="s">
@@ -1640,15 +1754,15 @@
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
+      <c r="C14" s="7" t="s">
         <v>92</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
+    <row r="15" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C15" s="7" t="s">
         <v>93</v>
       </c>
       <c r="D15" t="s">
@@ -1656,7 +1770,7 @@
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+      <c r="C16" s="7" t="s">
         <v>94</v>
       </c>
       <c r="D16" t="s">
@@ -1665,6 +1779,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
changes to Database per Adrian also update test excel
</commit_message>
<xml_diff>
--- a/Reports/Action List.xlsx
+++ b/Reports/Action List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Home Page" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,9 @@
     <sheet name="Profile Page 2" sheetId="5" r:id="rId6"/>
     <sheet name="Reports" sheetId="6" r:id="rId7"/>
     <sheet name="Testing Requirements" sheetId="7" r:id="rId8"/>
-    <sheet name="DatesGrade Structure" sheetId="8" r:id="rId9"/>
+    <sheet name="Test Data Creation notes" sheetId="11" r:id="rId9"/>
+    <sheet name="DatesGrade Structure" sheetId="8" r:id="rId10"/>
+    <sheet name="Sheet3" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="210">
   <si>
     <t xml:space="preserve">lot of informaiton -  </t>
   </si>
@@ -484,12 +486,230 @@
   <si>
     <t>none of the buttons in system  functional yet</t>
   </si>
+  <si>
+    <t>Section Marks Report 20% 
+Usability 20%
+ Registration 10%
+ Profiles 10%
+ Browse 10% 
+Search 15% 
+Auto-suggest 5%
+ Administration 10%
+ Extras Up 10% extra credit</t>
+  </si>
+  <si>
+    <t>logon as Lisa Sharp and like Angela.Martin</t>
+  </si>
+  <si>
+    <t>worked</t>
+  </si>
+  <si>
+    <t>test11</t>
+  </si>
+  <si>
+    <t>logon as as Angela.Marting - to check if Test 10  Lisa is someone interetsed in me</t>
+  </si>
+  <si>
+    <t>Angela appears as a match not interested in me</t>
+  </si>
+  <si>
+    <t>Adrian to check</t>
+  </si>
+  <si>
+    <t>Logon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logon Details  remembering previous emails </t>
+  </si>
+  <si>
+    <t>not remembering Lisa</t>
+  </si>
+  <si>
+    <t>Meeting Space</t>
+  </si>
+  <si>
+    <t>IF user selects someone - nothing happens unless the person they liked has liked them.</t>
+  </si>
+  <si>
+    <t>Make sure and create test data with Users who have already liked the person</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Action on test Data to do test</t>
+  </si>
+  <si>
+    <t>test 14</t>
+  </si>
+  <si>
+    <t>meeting space select people I may be interested in</t>
+  </si>
+  <si>
+    <t>test 15</t>
+  </si>
+  <si>
+    <t>allowed me to select and view profile</t>
+  </si>
+  <si>
+    <t>test 16</t>
+  </si>
+  <si>
+    <r>
+      <t>Aborted with error " A session had already been started - ignoring session_start() in C:\Users\User\Documents\GitHub\WebProject\Web\ViewMatchProfile.php on line </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF212529"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>18"</t>
+    </r>
+  </si>
+  <si>
+    <t>Logged on as john.doe@gmail.com 
+select someone I like and view profile and like on view profile</t>
+  </si>
+  <si>
+    <t>logon Option</t>
+  </si>
+  <si>
+    <t>Edit profile</t>
+  </si>
+  <si>
+    <t>select correct partner I want to meet</t>
+  </si>
+  <si>
+    <t>mathces found</t>
+  </si>
+  <si>
+    <t>see if I get the correct sex partner</t>
+  </si>
+  <si>
+    <t>buttons Funciton</t>
+  </si>
+  <si>
+    <t>TEst10</t>
+  </si>
+  <si>
+    <t>test12</t>
+  </si>
+  <si>
+    <t>Test13</t>
+  </si>
+  <si>
+    <t>check like button</t>
+  </si>
+  <si>
+    <t>interested in me test</t>
+  </si>
+  <si>
+    <t>remember login details</t>
+  </si>
+  <si>
+    <t>view someone I am interested in and like them</t>
+  </si>
+  <si>
+    <t>allows me to select</t>
+  </si>
+  <si>
+    <t>select someone I am interetsed in</t>
+  </si>
+  <si>
+    <t>selected someone I like</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logged on as john.doe@gmail.com  and liked Lucas 
+</t>
+  </si>
+  <si>
+    <t>logon/meeting Space</t>
+  </si>
+  <si>
+    <t>Check Database</t>
+  </si>
+  <si>
+    <t>Test 17</t>
+  </si>
+  <si>
+    <t>Check if Interetsed in me works</t>
+  </si>
+  <si>
+    <t>logged on bella.walsh - Una nash interested in me</t>
+  </si>
+  <si>
+    <t>check chat funtion</t>
+  </si>
+  <si>
+    <t>Test 18</t>
+  </si>
+  <si>
+    <t>Broke with error</t>
+  </si>
+  <si>
+    <t>Interested in Me</t>
+  </si>
+  <si>
+    <t>Please note following flow.  System Match, Intereseted in me, Chat</t>
+  </si>
+  <si>
+    <t>if you say goodbye on any of these they will not appear again</t>
+  </si>
+  <si>
+    <t>create Admin user</t>
+  </si>
+  <si>
+    <t>user profile has IS ADMINISTRATOR</t>
+  </si>
+  <si>
+    <t>test 19</t>
+  </si>
+  <si>
+    <t>Cap off 100KB on Image</t>
+  </si>
+  <si>
+    <t>test20</t>
+  </si>
+  <si>
+    <t>Admin User needs to go directly to Admin Screen</t>
+  </si>
+  <si>
+    <t>logon as  16230124@studentmail.ul.ie</t>
+  </si>
+  <si>
+    <t>went stratight to meeting space</t>
+  </si>
+  <si>
+    <t>test21</t>
+  </si>
+  <si>
+    <t>Admin User need to be able to look at all users reported</t>
+  </si>
+  <si>
+    <t>admin useer need to be able to supend account</t>
+  </si>
+  <si>
+    <t>Admins user need to be able to terminate account</t>
+  </si>
+  <si>
+    <t>Test22</t>
+  </si>
+  <si>
+    <t>Test23</t>
+  </si>
+  <si>
+    <t>admins need to be able to assign user as administrator</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -516,6 +736,14 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -537,7 +765,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -575,88 +803,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFE8E8E8"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFE8E8E8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFE8E8E8"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFE8E8E8"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFE8E8E8"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFE8E8E8"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFE8E8E8"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFE8E8E8"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFE8E8E8"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1000,8 +1156,136 @@
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="5" t="s">
         <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:I13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="48" customWidth="1"/>
+    <col min="9" max="9" width="53.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" ht="134.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -1011,227 +1295,466 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G17"/>
+  <dimension ref="B1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="50.5703125" customWidth="1"/>
-    <col min="4" max="4" width="41" customWidth="1"/>
-    <col min="5" max="5" width="50.5703125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="50.85546875" customWidth="1"/>
+    <col min="4" max="4" width="50.5703125" customWidth="1"/>
+    <col min="5" max="5" width="41" customWidth="1"/>
+    <col min="6" max="6" width="50.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D1" t="s">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
         <v>113</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>111</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>110</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>107</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>101</v>
-      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>101</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" t="s">
         <v>101</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>112</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>116</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>117</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
         <v>118</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>120</v>
       </c>
       <c r="C9" t="s">
+        <v>167</v>
+      </c>
+      <c r="D9" t="s">
         <v>121</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>124</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>123</v>
       </c>
       <c r="C11" t="s">
+        <v>168</v>
+      </c>
+      <c r="D11" t="s">
         <v>121</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>127</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="F11" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="F11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="90" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>126</v>
       </c>
       <c r="C12" t="s">
+        <v>168</v>
+      </c>
+      <c r="D12" t="s">
         <v>125</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>128</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="F12" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="F12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="135" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>132</v>
       </c>
       <c r="C13" t="s">
+        <v>168</v>
+      </c>
+      <c r="D13" t="s">
         <v>131</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>128</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="F13" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>134</v>
       </c>
       <c r="C14" t="s">
+        <v>169</v>
+      </c>
+      <c r="D14" t="s">
         <v>125</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>135</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="F14" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>6</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>138</v>
       </c>
       <c r="C15" t="s">
+        <v>170</v>
+      </c>
+      <c r="D15" t="s">
         <v>121</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>135</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="F15" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="F15" t="s">
-        <v>21</v>
-      </c>
       <c r="G15" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>141</v>
       </c>
       <c r="C16" t="s">
+        <v>171</v>
+      </c>
+      <c r="D16" t="s">
         <v>121</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>135</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="F16" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="F16" t="s">
-        <v>21</v>
-      </c>
       <c r="G16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>173</v>
+      </c>
       <c r="C17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D17" t="s">
         <v>143</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>135</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="F17" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="F17" t="s">
-        <v>21</v>
+      <c r="G17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>148</v>
+      </c>
+      <c r="C18" t="s">
+        <v>176</v>
+      </c>
+      <c r="D18" t="s">
+        <v>146</v>
+      </c>
+      <c r="E18" t="s">
+        <v>135</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>174</v>
+      </c>
+      <c r="C19" t="s">
+        <v>177</v>
+      </c>
+      <c r="D19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="G19" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>175</v>
+      </c>
+      <c r="C20" t="s">
+        <v>178</v>
+      </c>
+      <c r="D20" t="s">
+        <v>153</v>
+      </c>
+      <c r="E20" t="s">
+        <v>152</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="G20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>160</v>
+      </c>
+      <c r="C21" t="s">
+        <v>181</v>
+      </c>
+      <c r="D21" t="s">
+        <v>161</v>
+      </c>
+      <c r="E21" t="s">
+        <v>135</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="G21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>162</v>
+      </c>
+      <c r="C22" t="s">
+        <v>182</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E22" t="s">
+        <v>135</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="G22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>164</v>
+      </c>
+      <c r="C23" t="s">
+        <v>179</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E23" t="s">
+        <v>135</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="G23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>186</v>
+      </c>
+      <c r="C24" t="s">
+        <v>187</v>
+      </c>
+      <c r="D24" t="s">
+        <v>188</v>
+      </c>
+      <c r="E24" t="s">
+        <v>184</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>190</v>
+      </c>
+      <c r="C25" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>197</v>
+      </c>
+      <c r="C26" t="s">
+        <v>198</v>
+      </c>
+      <c r="G26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>199</v>
+      </c>
+      <c r="C27" t="s">
+        <v>200</v>
+      </c>
+      <c r="D27" t="s">
+        <v>201</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="G27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>203</v>
+      </c>
+      <c r="C28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>207</v>
+      </c>
+      <c r="C29" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>207</v>
+      </c>
+      <c r="C30" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>208</v>
+      </c>
+      <c r="C31" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -1245,7 +1768,7 @@
   <dimension ref="B2:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1665,12 +2188,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="83" style="7" customWidth="1"/>
+    <col min="3" max="3" width="83" style="3" customWidth="1"/>
     <col min="5" max="5" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D4" t="s">
@@ -1678,7 +2201,7 @@
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="3" t="s">
         <v>56</v>
       </c>
       <c r="D5" t="s">
@@ -1686,7 +2209,7 @@
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="3" t="s">
         <v>61</v>
       </c>
       <c r="D7" t="s">
@@ -1694,7 +2217,7 @@
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="3" t="s">
         <v>86</v>
       </c>
       <c r="D8" t="s">
@@ -1705,7 +2228,7 @@
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="3" t="s">
         <v>87</v>
       </c>
       <c r="D9" t="s">
@@ -1716,7 +2239,7 @@
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="3" t="s">
         <v>88</v>
       </c>
       <c r="D10" t="s">
@@ -1727,7 +2250,7 @@
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="3" t="s">
         <v>89</v>
       </c>
       <c r="D11" t="s">
@@ -1738,7 +2261,7 @@
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="3" t="s">
         <v>90</v>
       </c>
       <c r="D12" t="s">
@@ -1746,7 +2269,7 @@
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="3" t="s">
         <v>91</v>
       </c>
       <c r="D13" t="s">
@@ -1754,7 +2277,7 @@
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D14" t="s">
@@ -1762,7 +2285,7 @@
       </c>
     </row>
     <row r="15" spans="3:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="3" t="s">
         <v>93</v>
       </c>
       <c r="D15" t="s">
@@ -1770,7 +2293,7 @@
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="3" t="s">
         <v>94</v>
       </c>
       <c r="D16" t="s">
@@ -1787,18 +2310,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="110.140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="110.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="54.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="3" t="s">
         <v>57</v>
       </c>
       <c r="C3" t="s">
@@ -1806,7 +2329,7 @@
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C4" t="s">
@@ -1817,7 +2340,7 @@
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C6" t="s">
@@ -1825,7 +2348,7 @@
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C7" t="s">
@@ -1833,7 +2356,7 @@
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C8" t="s">
@@ -1841,7 +2364,7 @@
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C9" t="s">
@@ -1849,7 +2372,7 @@
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="3" t="s">
         <v>80</v>
       </c>
       <c r="C10" t="s">
@@ -1857,7 +2380,7 @@
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="3" t="s">
         <v>81</v>
       </c>
       <c r="C11" t="s">
@@ -1865,7 +2388,7 @@
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C12" t="s">
@@ -1873,7 +2396,7 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C13" t="s">
@@ -1881,7 +2404,7 @@
       </c>
     </row>
     <row r="14" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="3" t="s">
         <v>84</v>
       </c>
       <c r="C14" t="s">
@@ -1889,7 +2412,7 @@
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="3" t="s">
         <v>85</v>
       </c>
       <c r="C15" t="s">
@@ -1897,12 +2420,12 @@
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="3" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="4" t="s">
         <v>96</v>
       </c>
       <c r="C18" t="s">
@@ -1910,7 +2433,7 @@
       </c>
     </row>
     <row r="19" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="4" t="s">
         <v>97</v>
       </c>
       <c r="C19" t="s">
@@ -1918,7 +2441,7 @@
       </c>
     </row>
     <row r="20" spans="2:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C20" t="s">
@@ -1926,7 +2449,7 @@
       </c>
     </row>
     <row r="21" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="4" t="s">
         <v>99</v>
       </c>
       <c r="C21" t="s">
@@ -1934,7 +2457,7 @@
       </c>
     </row>
     <row r="22" spans="2:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="4" t="s">
         <v>100</v>
       </c>
       <c r="C22" t="s">
@@ -1949,85 +2472,53 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E13"/>
+  <dimension ref="B3:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="48" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="49" customWidth="1"/>
+    <col min="4" max="4" width="52.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" ht="77.25" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
-        <v>74</v>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C5" t="s">
+        <v>193</v>
+      </c>
+      <c r="D5" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated action list GITHUB, WEBPROJECT.ACTIONLIST
</commit_message>
<xml_diff>
--- a/Reports/Action List.xlsx
+++ b/Reports/Action List.xlsx
@@ -25,7 +25,7 @@
     <sheet name="Sheet3" sheetId="12" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Testing  Details '!$B$1:$H$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Testing  Details '!$B$1:$H$44</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="277">
   <si>
     <t xml:space="preserve">lot of informaiton -  </t>
   </si>
@@ -372,9 +372,6 @@
     <t xml:space="preserve">Menu not working </t>
   </si>
   <si>
-    <t xml:space="preserve">Forgot Password Option </t>
-  </si>
-  <si>
     <t>Allowed me to enter email but did not receive email</t>
   </si>
   <si>
@@ -390,9 +387,6 @@
     <t>Test2</t>
   </si>
   <si>
-    <t>Option</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -402,9 +396,6 @@
     <t>Logon as Lisa Sharp Password welcomE01#</t>
   </si>
   <si>
-    <t xml:space="preserve">allowed me to logon and took me to Meeting Space </t>
-  </si>
-  <si>
     <t>looks good so far</t>
   </si>
   <si>
@@ -420,19 +411,7 @@
     <t>Test4</t>
   </si>
   <si>
-    <t>Logon option</t>
-  </si>
-  <si>
-    <t>logon as Lisa Sharp</t>
-  </si>
-  <si>
     <t>test 5</t>
-  </si>
-  <si>
-    <t>Logon Option/Meting Space. Edit profile</t>
-  </si>
-  <si>
-    <t>Logon Option/Meeting Space/ Edit profile</t>
   </si>
   <si>
     <t>First screen work , second screen works until I press save and it abends
@@ -445,9 +424,6 @@
 </t>
   </si>
   <si>
-    <t>Logon as Carol.James@gmail.com Password WelcomeE01</t>
-  </si>
-  <si>
     <t>Test 6</t>
   </si>
   <si>
@@ -457,22 +433,13 @@
     <t>Test 7</t>
   </si>
   <si>
-    <t>logon/Meeting Space</t>
-  </si>
-  <si>
     <t>chatting with Paul even though she wants Female ?</t>
   </si>
   <si>
-    <t>Bad Data in Data base</t>
-  </si>
-  <si>
     <t>Test 8</t>
   </si>
   <si>
     <t xml:space="preserve">You are chatting with  No Mathces Found </t>
-  </si>
-  <si>
-    <t>Need clarify on message</t>
   </si>
   <si>
     <t>Test 9</t>
@@ -514,9 +481,6 @@
   </si>
   <si>
     <t>Adrian to check</t>
-  </si>
-  <si>
-    <t>Logon</t>
   </si>
   <si>
     <t xml:space="preserve">Logon Details  remembering previous emails </t>
@@ -575,12 +539,6 @@
 select someone I like and view profile and like on view profile</t>
   </si>
   <si>
-    <t>logon Option</t>
-  </si>
-  <si>
-    <t>Edit profile</t>
-  </si>
-  <si>
     <t>select correct partner I want to meet</t>
   </si>
   <si>
@@ -588,9 +546,6 @@
   </si>
   <si>
     <t>see if I get the correct sex partner</t>
-  </si>
-  <si>
-    <t>buttons Funciton</t>
   </si>
   <si>
     <t>TEst10</t>
@@ -627,9 +582,6 @@
 </t>
   </si>
   <si>
-    <t>logon/meeting Space</t>
-  </si>
-  <si>
     <t>Check Database</t>
   </si>
   <si>
@@ -702,9 +654,6 @@
     <t>Test24</t>
   </si>
   <si>
-    <t>to be created - Niall</t>
-  </si>
-  <si>
     <t>Admin need to be able to assign user as administrator</t>
   </si>
   <si>
@@ -723,9 +672,6 @@
     <t>correct all the open tests</t>
   </si>
   <si>
-    <t>Checked again on 25 July - Still error open</t>
-  </si>
-  <si>
     <t>Meeting Spaces Showing  Matches me with Carol James even though she only wants female partners, Hit View to View Carol Profile. Liked profile and got error</t>
   </si>
   <si>
@@ -823,6 +769,146 @@
   </si>
   <si>
     <t>Sent email to team</t>
+  </si>
+  <si>
+    <t>Test#</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Logon Details - Passwork Forgot</t>
+  </si>
+  <si>
+    <t>Adrian</t>
+  </si>
+  <si>
+    <t>Get onto Meeting Space from logon</t>
+  </si>
+  <si>
+    <t>Check If Edit Profile Works on Meeting Space</t>
+  </si>
+  <si>
+    <t>Check if save working on Edit Profile</t>
+  </si>
+  <si>
+    <t>Working now</t>
+  </si>
+  <si>
+    <t>Edit Porfile of another user</t>
+  </si>
+  <si>
+    <t>Edit Profile for Carol James</t>
+  </si>
+  <si>
+    <t>logon as Lisa Sharp- Logon Option/Meeting Space/ Edit profile</t>
+  </si>
+  <si>
+    <t>Logon as Carol.James@gmail.com Password WelcomeE01/Logon Option/Meeting Space/ Edit profile</t>
+  </si>
+  <si>
+    <t>logon as Lisa Sharp/meeting Space</t>
+  </si>
+  <si>
+    <t>Need to click on Photo</t>
+  </si>
+  <si>
+    <t>Logon as  Carol.James@gmail.com password welcomE01#/meeting space</t>
+  </si>
+  <si>
+    <t>Adrian/Mary</t>
+  </si>
+  <si>
+    <t>Niall</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Adrian ??</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>Test42</t>
+  </si>
+  <si>
+    <t>Register new user</t>
+  </si>
+  <si>
+    <t>Register, Patballycannon@gmail.com , Password submit</t>
+  </si>
+  <si>
+    <t>Got Error Notice: Undefined index: email in C:\Users\User\Documents\GitHub\WebProject\Web\Register.php on line 24</t>
+  </si>
+  <si>
+    <t>Adrian to check on 28 April</t>
+  </si>
+  <si>
+    <t>tried again not working 27/7</t>
+  </si>
+  <si>
+    <t>Test 43</t>
+  </si>
+  <si>
+    <t>Logon on throughHIVE -</t>
+  </si>
+  <si>
+    <t>Liaa Sharp</t>
+  </si>
+  <si>
+    <t>Bringing me to meeting space  - no photos for matches and duplicate buttons Like Like 
+http://hive.csis.ul.ie/4065/group05/MeetingSpace.php</t>
+  </si>
+  <si>
+    <t>OPen</t>
+  </si>
+  <si>
+    <t>Test 44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mary </t>
+  </si>
+  <si>
+    <t>Seeking Age Profile</t>
+  </si>
+  <si>
+    <t>Lisa Sharp - Seking Age  Profile. Saved details.  When in again Age is not saved on slider
+http://hive.csis.ul.ie/4065/group05/UpdateProfile.php</t>
+  </si>
+  <si>
+    <t>Checked again on 28  July - Still showing Male partners</t>
+  </si>
+  <si>
+    <t>same as Test 9 - Open</t>
+  </si>
+  <si>
+    <t>Slide bar always defaults back .  Deirdre to put in Doc</t>
+  </si>
+  <si>
+    <t>Looks Good Left Open until I validate correctly</t>
+  </si>
+  <si>
+    <t>buttons Functon in Meeting space</t>
+  </si>
+  <si>
+    <t>test 44</t>
+  </si>
+  <si>
+    <t>Check Age Slider - New uSer</t>
+  </si>
+  <si>
+    <t>PatBallycannon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Logged in ok but allowed me to edit profile and put in from 40 to 20 for seeking age</t>
   </si>
 </sst>
 </file>
@@ -1317,7 +1403,7 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1348,7 +1434,7 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="3" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>101</v>
@@ -1440,12 +1526,12 @@
   <sheetData>
     <row r="2" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -1455,404 +1541,438 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H41"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="B1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="47.7109375" customWidth="1"/>
-    <col min="4" max="4" width="50.5703125" customWidth="1"/>
-    <col min="5" max="5" width="41" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="50.5703125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="27.28515625" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D1" t="s">
+        <v>233</v>
+      </c>
       <c r="E1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="G1" t="s">
         <v>113</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="G1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" t="s">
+        <v>236</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>111</v>
       </c>
-      <c r="D2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>112</v>
+      <c r="C3" t="s">
+        <v>237</v>
       </c>
       <c r="D3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E3" t="s">
-        <v>117</v>
+        <v>236</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H3"/>
+    </row>
+    <row r="4" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C4" t="s">
-        <v>166</v>
+        <v>238</v>
       </c>
       <c r="D4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E4" t="s">
-        <v>123</v>
+        <v>236</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H4"/>
+    </row>
+    <row r="5" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C5" t="s">
-        <v>167</v>
+        <v>239</v>
       </c>
       <c r="D5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E5" t="s">
-        <v>126</v>
+        <v>236</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="G5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C6" t="s">
-        <v>167</v>
+        <v>241</v>
       </c>
       <c r="D6" t="s">
-        <v>124</v>
+        <v>243</v>
       </c>
       <c r="E6" t="s">
-        <v>127</v>
+        <v>236</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="G6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="H6"/>
+    </row>
+    <row r="7" spans="2:8" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C7" t="s">
-        <v>167</v>
+        <v>242</v>
       </c>
       <c r="D7" t="s">
-        <v>130</v>
+        <v>244</v>
       </c>
       <c r="E7" t="s">
-        <v>127</v>
+        <v>236</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="G7" t="s">
         <v>6</v>
       </c>
+      <c r="H7"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C8" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="D8" t="s">
-        <v>124</v>
+        <v>245</v>
       </c>
       <c r="E8" t="s">
-        <v>134</v>
+        <v>236</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="G8" t="s">
         <v>21</v>
       </c>
-      <c r="H8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H8" s="3" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C9" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="D9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E9" t="s">
-        <v>134</v>
+        <v>236</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="G9" t="s">
         <v>6</v>
       </c>
       <c r="H9" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="C10" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="D10" t="s">
-        <v>120</v>
+        <v>247</v>
       </c>
       <c r="E10" t="s">
+        <v>236</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>157</v>
+      </c>
+      <c r="C11" t="s">
+        <v>272</v>
+      </c>
+      <c r="D11" t="s">
+        <v>131</v>
+      </c>
+      <c r="E11" t="s">
+        <v>248</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12" t="s">
+        <v>160</v>
+      </c>
+      <c r="D12" t="s">
         <v>134</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="G10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>172</v>
-      </c>
-      <c r="C11" t="s">
-        <v>171</v>
-      </c>
-      <c r="D11" t="s">
-        <v>142</v>
-      </c>
-      <c r="E11" t="s">
-        <v>134</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="G11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>147</v>
-      </c>
-      <c r="C12" t="s">
-        <v>175</v>
-      </c>
-      <c r="D12" t="s">
-        <v>145</v>
-      </c>
       <c r="E12" t="s">
-        <v>134</v>
+        <v>236</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="G12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H12"/>
+    </row>
+    <row r="13" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="C13" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="D13" t="s">
-        <v>148</v>
+        <v>137</v>
+      </c>
+      <c r="E13" t="s">
+        <v>236</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="G13" t="s">
         <v>8</v>
       </c>
       <c r="H13" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="D14" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="E14" t="s">
-        <v>151</v>
+        <v>236</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="G14" t="s">
         <v>8</v>
       </c>
       <c r="H14" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C15" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="D15" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="E15" t="s">
-        <v>134</v>
+        <v>248</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="G15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H15"/>
+    </row>
+    <row r="16" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="C16" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="E16" t="s">
-        <v>134</v>
+        <v>248</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="G16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="H16"/>
+    </row>
+    <row r="17" spans="2:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
+        <v>151</v>
+      </c>
+      <c r="C17" t="s">
         <v>163</v>
       </c>
-      <c r="C17" t="s">
-        <v>178</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="E17" t="s">
-        <v>134</v>
+        <v>248</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="G17" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H17"/>
+    </row>
+    <row r="18" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="C18" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="D18" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="E18" t="s">
-        <v>183</v>
+        <v>236</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="G18" t="s">
         <v>6</v>
       </c>
       <c r="H18" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="C19" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="G19" t="s">
         <v>21</v>
       </c>
-      <c r="H19" t="s">
-        <v>245</v>
+      <c r="H19" s="3" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C20" t="s">
-        <v>197</v>
+        <v>181</v>
+      </c>
+      <c r="E20" t="s">
+        <v>248</v>
       </c>
       <c r="G20" t="s">
         <v>21</v>
@@ -1860,19 +1980,19 @@
     </row>
     <row r="21" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="C21" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="D21" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="E21" t="s">
-        <v>101</v>
+        <v>249</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="G21" t="s">
         <v>21</v>
@@ -1880,16 +2000,16 @@
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="C22" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="D22" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="E22" t="s">
-        <v>208</v>
+        <v>249</v>
       </c>
       <c r="G22" t="s">
         <v>21</v>
@@ -1897,16 +2017,16 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="C23" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="D23" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="E23" t="s">
-        <v>208</v>
+        <v>249</v>
       </c>
       <c r="G23" t="s">
         <v>21</v>
@@ -1914,16 +2034,16 @@
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="C24" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="D24" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="E24" t="s">
-        <v>208</v>
+        <v>249</v>
       </c>
       <c r="G24" t="s">
         <v>21</v>
@@ -1931,16 +2051,16 @@
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="C25" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
       <c r="D25" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="E25" t="s">
-        <v>208</v>
+        <v>249</v>
       </c>
       <c r="G25" t="s">
         <v>21</v>
@@ -1948,146 +2068,334 @@
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="C26" t="s">
-        <v>211</v>
+        <v>194</v>
+      </c>
+      <c r="E26" t="s">
+        <v>249</v>
+      </c>
+      <c r="G26" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="C27" t="s">
-        <v>212</v>
+        <v>195</v>
+      </c>
+      <c r="E27" t="s">
+        <v>250</v>
+      </c>
+      <c r="G27" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="C28" t="s">
-        <v>233</v>
+        <v>215</v>
+      </c>
+      <c r="E28" t="s">
+        <v>251</v>
+      </c>
+      <c r="G28" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="C29" t="s">
-        <v>213</v>
+        <v>196</v>
+      </c>
+      <c r="E29" t="s">
+        <v>250</v>
+      </c>
+      <c r="G29" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="C30" t="s">
-        <v>214</v>
+        <v>197</v>
+      </c>
+      <c r="E30" t="s">
+        <v>252</v>
+      </c>
+      <c r="G30" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>235</v>
+        <v>217</v>
+      </c>
+      <c r="E31" t="s">
+        <v>249</v>
+      </c>
+      <c r="G31" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>219</v>
+        <v>201</v>
+      </c>
+      <c r="E32" t="s">
+        <v>236</v>
+      </c>
+      <c r="G32" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
+        <v>218</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="E33" t="s">
         <v>236</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>220</v>
+      <c r="G33" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>221</v>
+        <v>203</v>
+      </c>
+      <c r="E34" t="s">
+        <v>236</v>
+      </c>
+      <c r="G34" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>222</v>
+        <v>204</v>
+      </c>
+      <c r="E35" t="s">
+        <v>236</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="G35" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>223</v>
+        <v>205</v>
+      </c>
+      <c r="E36" t="s">
+        <v>236</v>
+      </c>
+      <c r="G36" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>224</v>
+        <v>206</v>
+      </c>
+      <c r="E37" t="s">
+        <v>236</v>
+      </c>
+      <c r="G37" t="s">
+        <v>21</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>225</v>
+        <v>207</v>
+      </c>
+      <c r="E38" t="s">
+        <v>236</v>
+      </c>
+      <c r="G38" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>226</v>
+        <v>208</v>
+      </c>
+      <c r="E39" t="s">
+        <v>236</v>
+      </c>
+      <c r="G39" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>227</v>
+        <v>209</v>
+      </c>
+      <c r="E40" t="s">
+        <v>249</v>
+      </c>
+      <c r="G40" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="C41" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="D41" t="s">
-        <v>142</v>
+        <v>131</v>
+      </c>
+      <c r="E41" t="s">
+        <v>236</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="G41" t="s">
         <v>21</v>
       </c>
-      <c r="H41" t="s">
-        <v>248</v>
+      <c r="H41" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>253</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="D42" t="s">
+        <v>255</v>
+      </c>
+      <c r="E42" t="s">
+        <v>236</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="G42" t="s">
+        <v>21</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>259</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="D43" t="s">
+        <v>261</v>
+      </c>
+      <c r="E43" t="s">
+        <v>251</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="G43" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" ht="120" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>264</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E44" t="s">
+        <v>265</v>
+      </c>
+      <c r="G44" t="s">
+        <v>8</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>273</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="D45" t="s">
+        <v>275</v>
+      </c>
+      <c r="E45" t="s">
+        <v>250</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="G45" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:H41"/>
+  <autoFilter ref="B1:H44">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="Open"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2817,21 +3125,21 @@
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="D3" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C4" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="D4" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="E4" t="s">
         <v>101</v>
@@ -2839,13 +3147,13 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="C5" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="D5" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates on action list
</commit_message>
<xml_diff>
--- a/Reports/Action List.xlsx
+++ b/Reports/Action List.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="281">
   <si>
     <t xml:space="preserve">lot of informaiton -  </t>
   </si>
@@ -909,6 +909,18 @@
   </si>
   <si>
     <t xml:space="preserve"> Logged in ok but allowed me to edit profile and put in from 40 to 20 for seeking age</t>
+  </si>
+  <si>
+    <t>test45</t>
+  </si>
+  <si>
+    <t>Carol.James@gmail.com password welcomE01#/meeting space</t>
+  </si>
+  <si>
+    <t>does not remember email when I go back to site</t>
+  </si>
+  <si>
+    <t>Can App remember email when I go back from Meeting space</t>
   </si>
 </sst>
 </file>
@@ -1542,17 +1554,17 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="B1:H45"/>
+  <dimension ref="B1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="47.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="50.5703125" style="3" customWidth="1"/>
     <col min="8" max="8" width="27.28515625" style="3" customWidth="1"/>
@@ -1565,7 +1577,7 @@
       <c r="C1" t="s">
         <v>232</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>233</v>
       </c>
       <c r="E1" t="s">
@@ -1578,14 +1590,14 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>110</v>
       </c>
       <c r="C2" t="s">
         <v>235</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>109</v>
       </c>
       <c r="E2" t="s">
@@ -1705,14 +1717,14 @@
       </c>
       <c r="H7"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>125</v>
       </c>
       <c r="C8" t="s">
         <v>154</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>245</v>
       </c>
       <c r="E8" t="s">
@@ -1751,14 +1763,14 @@
         <v>246</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>129</v>
       </c>
       <c r="C10" t="s">
         <v>156</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
         <v>247</v>
       </c>
       <c r="E10" t="s">
@@ -1774,14 +1786,14 @@
         <v>268</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>157</v>
       </c>
       <c r="C11" t="s">
         <v>272</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="3" t="s">
         <v>131</v>
       </c>
       <c r="E11" t="s">
@@ -1985,7 +1997,7 @@
       <c r="C21" t="s">
         <v>183</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="3" t="s">
         <v>184</v>
       </c>
       <c r="E21" t="s">
@@ -1998,14 +2010,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>185</v>
       </c>
       <c r="C22" t="s">
         <v>186</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="3" t="s">
         <v>184</v>
       </c>
       <c r="E22" t="s">
@@ -2015,14 +2027,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>189</v>
       </c>
       <c r="C23" t="s">
         <v>187</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="3" t="s">
         <v>184</v>
       </c>
       <c r="E23" t="s">
@@ -2032,14 +2044,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>190</v>
       </c>
       <c r="C24" t="s">
         <v>188</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="3" t="s">
         <v>184</v>
       </c>
       <c r="E24" t="s">
@@ -2049,14 +2061,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>191</v>
       </c>
       <c r="C25" t="s">
         <v>192</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="3" t="s">
         <v>184</v>
       </c>
       <c r="E25" t="s">
@@ -2282,14 +2294,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>228</v>
       </c>
       <c r="C41" t="s">
         <v>229</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="3" t="s">
         <v>131</v>
       </c>
       <c r="E41" t="s">
@@ -2305,14 +2317,14 @@
         <v>230</v>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>253</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="3" t="s">
         <v>255</v>
       </c>
       <c r="E42" t="s">
@@ -2335,7 +2347,7 @@
       <c r="C43" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="3" t="s">
         <v>261</v>
       </c>
       <c r="E43" t="s">
@@ -2375,7 +2387,7 @@
       <c r="C45" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="3" t="s">
         <v>275</v>
       </c>
       <c r="E45" t="s">
@@ -2385,6 +2397,26 @@
         <v>276</v>
       </c>
       <c r="G45" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>277</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="E46" t="s">
+        <v>236</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="G46" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added clarification sheet to discuss with Adrian, also open issue remain same
</commit_message>
<xml_diff>
--- a/Reports/Action List.xlsx
+++ b/Reports/Action List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="8" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="7" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Home Page" sheetId="2" r:id="rId1"/>
@@ -20,10 +20,10 @@
     <sheet name="Profile Page 2" sheetId="5" r:id="rId6"/>
     <sheet name="Reports" sheetId="6" r:id="rId7"/>
     <sheet name="Testing Requirements" sheetId="7" r:id="rId8"/>
-    <sheet name="Test Data Creation notes" sheetId="11" r:id="rId9"/>
-    <sheet name="DatesGrade Structure" sheetId="8" r:id="rId10"/>
-    <sheet name="Functionality" sheetId="16" r:id="rId11"/>
-    <sheet name="Sheet6" sheetId="17" r:id="rId12"/>
+    <sheet name="DatesGrade Structure" sheetId="8" r:id="rId9"/>
+    <sheet name="Functionality" sheetId="16" r:id="rId10"/>
+    <sheet name="Sheet6" sheetId="17" r:id="rId11"/>
+    <sheet name="Clarification" sheetId="18" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Testing  Details '!$B$1:$H$57</definedName>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="433">
   <si>
     <t xml:space="preserve">lot of informaiton -  </t>
   </si>
@@ -493,18 +493,6 @@
     <t>Meeting Space</t>
   </si>
   <si>
-    <t>IF user selects someone - nothing happens unless the person they liked has liked them.</t>
-  </si>
-  <si>
-    <t>Make sure and create test data with Users who have already liked the person</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>Action on test Data to do test</t>
-  </si>
-  <si>
     <t>test 14</t>
   </si>
   <si>
@@ -604,15 +592,6 @@
     <t>Broke with error</t>
   </si>
   <si>
-    <t>Interested in Me</t>
-  </si>
-  <si>
-    <t>Please note following flow.  System Match, Intereseted in me, Chat</t>
-  </si>
-  <si>
-    <t>if you say goodbye on any of these they will not appear again</t>
-  </si>
-  <si>
     <t>test 19</t>
   </si>
   <si>
@@ -1992,6 +1971,48 @@
   </si>
   <si>
     <t>Deirdre to recheck</t>
+  </si>
+  <si>
+    <t>FN5.105</t>
+  </si>
+  <si>
+    <t>Black list of words</t>
+  </si>
+  <si>
+    <t>Black  List words</t>
+  </si>
+  <si>
+    <t>How can SYSADMIN  add additional words to Data Base</t>
+  </si>
+  <si>
+    <t>How can sysadmin check what is on the profile with Black list words</t>
+  </si>
+  <si>
+    <t>Sys Admin Login</t>
+  </si>
+  <si>
+    <t>When user logs on they are taken to list of people  with issues
+What does the wee circle at the side of the photo mean ?
+IF you select photo the wee circle also is  flagged
+Why would the same person be there a number of times ?</t>
+  </si>
+  <si>
+    <t>How can I validate if someone is suspended -</t>
+  </si>
+  <si>
+    <t>How can you unsuspend a account ?</t>
+  </si>
+  <si>
+    <t>BAR ?  I  selected uset and flagged as BAR but nothing happened .
+Is user supposed to disappear from screen ?</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3 ways  flag Inappropriate behaviours
+1. User can report someone for inappropriate behaviours 
+2. Which screen has code in the background  to check inappropriate code</t>
   </si>
 </sst>
 </file>
@@ -2374,7 +2395,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -2485,6 +2506,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2512,9 +2536,11 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2861,110 +2887,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I13"/>
+  <dimension ref="B3:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="5" max="5" width="48" customWidth="1"/>
-    <col min="9" max="9" width="53.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:9" ht="134.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E31"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2977,24 +2903,24 @@
   <sheetData>
     <row r="3" spans="2:5" ht="21" x14ac:dyDescent="0.25">
       <c r="B3" s="26" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="37" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="E4" t="s">
         <v>101</v>
@@ -3002,80 +2928,80 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="29" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="29" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="41" t="s">
-        <v>286</v>
-      </c>
-      <c r="C7" s="38" t="s">
+      <c r="B7" s="42" t="s">
+        <v>279</v>
+      </c>
+      <c r="C7" s="39" t="s">
         <v>142</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="42"/>
-      <c r="C8" s="39"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="40"/>
       <c r="D8" s="30" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="42"/>
-      <c r="C9" s="39"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="40"/>
       <c r="D9" s="30" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="E9" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="42"/>
-      <c r="C10" s="39"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="40"/>
       <c r="D10" s="32" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="E10" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="42"/>
-      <c r="C11" s="39"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="40"/>
       <c r="D11" s="32" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="E11" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="43"/>
-      <c r="C12" s="40"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="41"/>
       <c r="D12" s="32" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="E12" t="s">
         <v>101</v>
@@ -3083,211 +3009,219 @@
     </row>
     <row r="13" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B13" s="29" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="29" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="D14" s="33" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="29" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B16" s="29" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" s="29" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="29" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="29" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="29" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B21" s="29" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="29" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="29" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="29" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="29" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="29" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="29" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="29" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="29" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="29" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="34" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="C31" s="35" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="D31" s="36" t="s">
-        <v>380</v>
+        <v>373</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>422</v>
       </c>
     </row>
   </sheetData>
@@ -3300,7 +3234,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
@@ -3318,379 +3252,379 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="44" t="s">
-        <v>388</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="46"/>
+      <c r="A1" s="45" t="s">
+        <v>381</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="47"/>
     </row>
     <row r="2" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>417</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>385</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>387</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>388</v>
+      </c>
+      <c r="I2" s="13" t="s">
         <v>389</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="J2" s="14" t="s">
         <v>390</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>424</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>391</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>392</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>393</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>394</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>395</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>396</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="17" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="17" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="J4" s="18" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="17" t="s">
+        <v>393</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>393</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>393</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>393</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>393</v>
+      </c>
+      <c r="I5" s="17" t="s">
         <v>400</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>400</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>400</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>400</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>400</v>
-      </c>
-      <c r="I5" s="17" t="s">
-        <v>407</v>
-      </c>
       <c r="J5" s="18" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="17" t="s">
+        <v>393</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>393</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>393</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>395</v>
+      </c>
+      <c r="H6" s="17" t="s">
         <v>400</v>
       </c>
-      <c r="E6" s="17" t="s">
-        <v>400</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>400</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>402</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>407</v>
-      </c>
       <c r="I6" s="17" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="C7" s="19"/>
       <c r="D7" s="17" t="s">
+        <v>393</v>
+      </c>
+      <c r="E7" s="17" t="s">
         <v>400</v>
       </c>
-      <c r="E7" s="17" t="s">
-        <v>407</v>
-      </c>
       <c r="F7" s="17" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="17" t="s">
+        <v>393</v>
+      </c>
+      <c r="E8" s="17" t="s">
         <v>400</v>
       </c>
-      <c r="E8" s="17" t="s">
-        <v>407</v>
-      </c>
       <c r="F8" s="17" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="17" t="s">
+        <v>393</v>
+      </c>
+      <c r="E9" s="17" t="s">
         <v>400</v>
       </c>
-      <c r="E9" s="17" t="s">
-        <v>407</v>
-      </c>
       <c r="F9" s="17" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="17" t="s">
+        <v>393</v>
+      </c>
+      <c r="E10" s="17" t="s">
         <v>400</v>
       </c>
-      <c r="E10" s="17" t="s">
-        <v>407</v>
-      </c>
       <c r="F10" s="17" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="17" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="17" t="s">
+        <v>393</v>
+      </c>
+      <c r="E12" s="17" t="s">
         <v>400</v>
       </c>
-      <c r="E12" s="17" t="s">
-        <v>407</v>
-      </c>
       <c r="F12" s="17" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="C13" s="22"/>
       <c r="D13" s="23" t="s">
+        <v>393</v>
+      </c>
+      <c r="E13" s="23" t="s">
         <v>400</v>
       </c>
-      <c r="E13" s="23" t="s">
-        <v>407</v>
-      </c>
       <c r="F13" s="23" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="H13" s="23" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="I13" s="23" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="J13" s="24" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -3705,6 +3639,81 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="66.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="48" t="s">
+        <v>423</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C4" s="48" t="s">
+        <v>423</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="48" t="s">
+        <v>423</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="C6" s="50" t="s">
+        <v>431</v>
+      </c>
+      <c r="D6" s="49" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="48" t="s">
+        <v>426</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="48" t="s">
+        <v>426</v>
+      </c>
+      <c r="D8" s="49" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C9" s="48" t="s">
+        <v>426</v>
+      </c>
+      <c r="D9" s="49" t="s">
+        <v>430</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
@@ -3712,7 +3721,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3726,16 +3735,16 @@
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="C1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="E1" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>112</v>
@@ -3749,13 +3758,13 @@
         <v>110</v>
       </c>
       <c r="C2" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>109</v>
       </c>
       <c r="E2" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>107</v>
@@ -3764,7 +3773,7 @@
         <v>21</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="3" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
@@ -3772,13 +3781,13 @@
         <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D3" t="s">
         <v>114</v>
       </c>
       <c r="E3" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>115</v>
@@ -3793,13 +3802,13 @@
         <v>116</v>
       </c>
       <c r="C4" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="D4" t="s">
         <v>117</v>
       </c>
       <c r="E4" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>118</v>
@@ -3814,13 +3823,13 @@
         <v>119</v>
       </c>
       <c r="C5" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="D5" t="s">
         <v>117</v>
       </c>
       <c r="E5" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>124</v>
@@ -3829,7 +3838,7 @@
         <v>6</v>
       </c>
       <c r="H5" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="90" hidden="1" x14ac:dyDescent="0.25">
@@ -3837,13 +3846,13 @@
         <v>120</v>
       </c>
       <c r="C6" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="D6" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E6" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>121</v>
@@ -3858,13 +3867,13 @@
         <v>123</v>
       </c>
       <c r="C7" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="D7" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E7" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>122</v>
@@ -3879,13 +3888,13 @@
         <v>125</v>
       </c>
       <c r="C8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="E8" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>126</v>
@@ -3894,7 +3903,7 @@
         <v>22</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
     </row>
     <row r="9" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
@@ -3902,13 +3911,13 @@
         <v>127</v>
       </c>
       <c r="C9" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D9" t="s">
         <v>117</v>
       </c>
       <c r="E9" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>128</v>
@@ -3917,7 +3926,7 @@
         <v>6</v>
       </c>
       <c r="H9" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -3925,13 +3934,13 @@
         <v>129</v>
       </c>
       <c r="C10" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E10" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>130</v>
@@ -3940,21 +3949,21 @@
         <v>6</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C11" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>131</v>
       </c>
       <c r="E11" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>132</v>
@@ -3963,7 +3972,7 @@
         <v>6</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
@@ -3971,13 +3980,13 @@
         <v>136</v>
       </c>
       <c r="C12" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D12" t="s">
         <v>134</v>
       </c>
       <c r="E12" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>135</v>
@@ -3989,16 +3998,16 @@
     </row>
     <row r="13" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C13" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D13" t="s">
         <v>137</v>
       </c>
       <c r="E13" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>138</v>
@@ -4007,21 +4016,21 @@
         <v>8</v>
       </c>
       <c r="H13" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D14" t="s">
         <v>140</v>
       </c>
       <c r="E14" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>141</v>
@@ -4035,19 +4044,19 @@
     </row>
     <row r="15" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C15" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D15" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E15" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="G15" t="s">
         <v>6</v>
@@ -4056,19 +4065,19 @@
     </row>
     <row r="16" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C16" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E16" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G16" t="s">
         <v>6</v>
@@ -4077,19 +4086,19 @@
     </row>
     <row r="17" spans="2:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C17" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E17" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="G17" t="s">
         <v>8</v>
@@ -4098,50 +4107,50 @@
     </row>
     <row r="18" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E18" t="s">
+        <v>227</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="D18" t="s">
-        <v>171</v>
-      </c>
-      <c r="E18" t="s">
-        <v>234</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>174</v>
       </c>
       <c r="G18" t="s">
         <v>6</v>
       </c>
       <c r="H18" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C19" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="G19" t="s">
         <v>6</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C20" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E20" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="G20" t="s">
         <v>21</v>
@@ -4149,19 +4158,19 @@
     </row>
     <row r="21" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C21" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="E21" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="G21" t="s">
         <v>21</v>
@@ -4169,16 +4178,16 @@
     </row>
     <row r="22" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="C22" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="E22" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="G22" t="s">
         <v>21</v>
@@ -4186,16 +4195,16 @@
     </row>
     <row r="23" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C23" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="E23" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="G23" t="s">
         <v>21</v>
@@ -4203,16 +4212,16 @@
     </row>
     <row r="24" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C24" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="E24" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="G24" t="s">
         <v>21</v>
@@ -4220,16 +4229,16 @@
     </row>
     <row r="25" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="C25" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="E25" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="G25" t="s">
         <v>21</v>
@@ -4237,13 +4246,13 @@
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C26" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="E26" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="G26" t="s">
         <v>21</v>
@@ -4251,13 +4260,13 @@
     </row>
     <row r="27" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C27" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="E27" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="G27" t="s">
         <v>8</v>
@@ -4265,13 +4274,13 @@
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C28" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="E28" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="G28" t="s">
         <v>21</v>
@@ -4279,13 +4288,13 @@
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C29" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="E29" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="G29" t="s">
         <v>21</v>
@@ -4293,13 +4302,13 @@
     </row>
     <row r="30" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C30" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="E30" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="G30" t="s">
         <v>8</v>
@@ -4307,13 +4316,13 @@
     </row>
     <row r="31" spans="2:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="E31" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="G31" t="s">
         <v>6</v>
@@ -4321,13 +4330,13 @@
     </row>
     <row r="32" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="E32" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="G32" t="s">
         <v>21</v>
@@ -4335,13 +4344,13 @@
     </row>
     <row r="33" spans="2:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="E33" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="G33" t="s">
         <v>6</v>
@@ -4349,13 +4358,13 @@
     </row>
     <row r="34" spans="2:8" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="E34" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="G34" t="s">
         <v>6</v>
@@ -4363,16 +4372,16 @@
     </row>
     <row r="35" spans="2:8" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E35" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="G35" t="s">
         <v>6</v>
@@ -4380,13 +4389,13 @@
     </row>
     <row r="36" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="E36" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="G36" t="s">
         <v>21</v>
@@ -4394,30 +4403,30 @@
     </row>
     <row r="37" spans="2:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="E37" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="G37" t="s">
         <v>6</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="E38" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="G38" t="s">
         <v>21</v>
@@ -4425,13 +4434,13 @@
     </row>
     <row r="39" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="E39" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="G39" t="s">
         <v>21</v>
@@ -4439,13 +4448,13 @@
     </row>
     <row r="40" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="E40" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="G40" t="s">
         <v>21</v>
@@ -4453,65 +4462,65 @@
     </row>
     <row r="41" spans="2:8" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="C41" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>131</v>
       </c>
       <c r="E41" t="s">
-        <v>234</v>
-      </c>
-      <c r="F41" s="47" t="s">
-        <v>196</v>
+        <v>227</v>
+      </c>
+      <c r="F41" s="38" t="s">
+        <v>189</v>
       </c>
       <c r="G41" t="s">
         <v>6</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="42" spans="2:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="E42" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="G42" t="s">
         <v>6</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="43" spans="2:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="E43" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="G43" t="s">
         <v>8</v>
@@ -4519,39 +4528,39 @@
     </row>
     <row r="44" spans="2:8" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="E44" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="G44" t="s">
         <v>8</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="45" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="E45" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="G45" t="s">
         <v>6</v>
@@ -4559,19 +4568,19 @@
     </row>
     <row r="46" spans="2:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="E46" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="G46" t="s">
         <v>6</v>
@@ -4579,36 +4588,36 @@
     </row>
     <row r="47" spans="2:8" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="E47" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="G47" t="s">
         <v>6</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
     </row>
     <row r="48" spans="2:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="G48" t="s">
         <v>6</v>
@@ -4616,19 +4625,19 @@
     </row>
     <row r="49" spans="2:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="E49" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="G49" t="s">
         <v>8</v>
@@ -4636,64 +4645,64 @@
     </row>
     <row r="50" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="G50" t="s">
         <v>59</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
     </row>
     <row r="51" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="G51" t="s">
         <v>21</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
     </row>
     <row r="52" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="G52" t="s">
         <v>21</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
     </row>
     <row r="53" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="G53" t="s">
         <v>21</v>
@@ -4701,13 +4710,13 @@
     </row>
     <row r="54" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="G54" t="s">
         <v>21</v>
@@ -4715,27 +4724,27 @@
     </row>
     <row r="55" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="G55" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="2:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="C56" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="D56" s="3" t="s">
         <v>365</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>372</v>
       </c>
       <c r="G56" t="s">
         <v>21</v>
@@ -4743,13 +4752,13 @@
     </row>
     <row r="57" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="G57" t="s">
         <v>21</v>
@@ -5481,53 +5490,100 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E5"/>
+  <dimension ref="B2:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="49" customWidth="1"/>
-    <col min="4" max="4" width="52.140625" customWidth="1"/>
+    <col min="5" max="5" width="48" customWidth="1"/>
+    <col min="9" max="9" width="53.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" ht="134.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
       <c r="C3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="E3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>142</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>143</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
-        <v>144</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>175</v>
-      </c>
-      <c r="C5" t="s">
-        <v>176</v>
-      </c>
-      <c r="D5" t="s">
-        <v>177</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
latest updates to Draft Report
</commit_message>
<xml_diff>
--- a/Reports/Action List.xlsx
+++ b/Reports/Action List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="7" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="8" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Home Page" sheetId="2" r:id="rId1"/>
@@ -22,8 +22,8 @@
     <sheet name="Testing Requirements" sheetId="7" r:id="rId8"/>
     <sheet name="DatesGrade Structure" sheetId="8" r:id="rId9"/>
     <sheet name="Functionality" sheetId="16" r:id="rId10"/>
-    <sheet name="Sheet6" sheetId="17" r:id="rId11"/>
-    <sheet name="Clarification" sheetId="18" r:id="rId12"/>
+    <sheet name="Clarification" sheetId="18" r:id="rId11"/>
+    <sheet name="logon&amp;passwords" sheetId="19" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Testing  Details '!$B$1:$H$57</definedName>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="405">
   <si>
     <t xml:space="preserve">lot of informaiton -  </t>
   </si>
@@ -1853,120 +1853,6 @@
     <t>This screen is initiated from the meeting space screen.  User can send message to proposed match and start conversations and visa versa</t>
   </si>
   <si>
-    <t>Future Partner  Website Project Status</t>
-  </si>
-  <si>
-    <t>Dating Pages</t>
-  </si>
-  <si>
-    <t>Page Link</t>
-  </si>
-  <si>
-    <t>Basic Screen Layout Complete</t>
-  </si>
-  <si>
-    <t>Layout fully compelte</t>
-  </si>
-  <si>
-    <t>accessing Database</t>
-  </si>
-  <si>
-    <t>Updating Database</t>
-  </si>
-  <si>
-    <t>All buttons functioning</t>
-  </si>
-  <si>
-    <t>Validation Complete</t>
-  </si>
-  <si>
-    <t>Style Complete</t>
-  </si>
-  <si>
-    <t>Index.php</t>
-  </si>
-  <si>
-    <t>http://hive.csis.ul.ie/4065/group05/index.php</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Logon.php</t>
-  </si>
-  <si>
-    <t>http://hive.csis.ul.ie/4065/group05/Logon.php</t>
-  </si>
-  <si>
-    <t>Register.php</t>
-  </si>
-  <si>
-    <t>http://hive.csis.ul.ie/4065/group05/Register.php</t>
-  </si>
-  <si>
-    <t>WIP</t>
-  </si>
-  <si>
-    <t>meetingspace.php</t>
-  </si>
-  <si>
-    <t>http://hive.csis.ul.ie/4065/group05/MeetingSpace.php</t>
-  </si>
-  <si>
-    <t>updateprofile.php</t>
-  </si>
-  <si>
-    <t>http://hive.csis.ul.ie/4065/group05/UpdateProfile.php</t>
-  </si>
-  <si>
-    <t>viewmatchprofile.php</t>
-  </si>
-  <si>
-    <t>http://hive.csis.ul.ie/4065/group05/ViewMatchProfile.php</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chatline.php                </t>
-  </si>
-  <si>
-    <t>http://hive.csis.ul.ie/4065/group05/ChatLine.php</t>
-  </si>
-  <si>
-    <t xml:space="preserve">matchfind.php               </t>
-  </si>
-  <si>
-    <t>http://hive.csis.ul.ie/4065/group05/MatchFind.php</t>
-  </si>
-  <si>
-    <t>removeaccount.php</t>
-  </si>
-  <si>
-    <t>http://hive.csis.ul.ie/4065/group05/RemoveAccount.php</t>
-  </si>
-  <si>
-    <t xml:space="preserve">passwordreset .php  </t>
-  </si>
-  <si>
-    <t>http://hive.csis.ul.ie/4065/group05/PasswordReset.php</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adminscreen.php             </t>
-  </si>
-  <si>
-    <t>Np</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>http://hive.csis.ul.ie/4065/group05/AdminScreen.php</t>
-  </si>
-  <si>
     <t>Adrian still working to perfection</t>
   </si>
   <si>
@@ -2013,13 +1899,43 @@
     <t xml:space="preserve"> 3 ways  flag Inappropriate behaviours
 1. User can report someone for inappropriate behaviours 
 2. Which screen has code in the background  to check inappropriate code</t>
+  </si>
+  <si>
+    <t>16230256@Studentmail.ul.ie</t>
+  </si>
+  <si>
+    <t>SysAdmin</t>
+  </si>
+  <si>
+    <t>welcomE01#</t>
+  </si>
+  <si>
+    <t>16230124@studentmail.ul.ie</t>
+  </si>
+  <si>
+    <t>mary's Logon wrong on Systadmin  Database upload -</t>
+  </si>
+  <si>
+    <t>0510661@stedentmail.ul.ie</t>
+  </si>
+  <si>
+    <t>0199124@studentmail.ul.ie</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>USER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2092,20 +2008,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="22"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="16"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -2151,7 +2053,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -2320,43 +2222,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -2395,7 +2260,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -2425,52 +2290,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2509,6 +2335,11 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2518,29 +2349,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2902,24 +2719,24 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="13" t="s">
         <v>371</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="13" t="s">
         <v>372</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="13" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="24" t="s">
         <v>275</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="15" t="s">
         <v>276</v>
       </c>
       <c r="E4" t="s">
@@ -2927,50 +2744,50 @@
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="16" t="s">
         <v>277</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="14" t="s">
         <v>269</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="15" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="16" t="s">
         <v>278</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="17" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="32" t="s">
         <v>279</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="18" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="43"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="30" t="s">
+      <c r="B8" s="33"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="17" t="s">
         <v>374</v>
       </c>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="43"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="30" t="s">
+      <c r="B9" s="33"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="17" t="s">
         <v>284</v>
       </c>
       <c r="E9" t="s">
@@ -2978,9 +2795,9 @@
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="43"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="32" t="s">
+      <c r="B10" s="33"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="19" t="s">
         <v>302</v>
       </c>
       <c r="E10" t="s">
@@ -2988,9 +2805,9 @@
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="43"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="32" t="s">
+      <c r="B11" s="33"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="19" t="s">
         <v>285</v>
       </c>
       <c r="E11" t="s">
@@ -2998,9 +2815,9 @@
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="44"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="32" t="s">
+      <c r="B12" s="34"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="19" t="s">
         <v>303</v>
       </c>
       <c r="E12" t="s">
@@ -3008,220 +2825,220 @@
       </c>
     </row>
     <row r="13" spans="2:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="16" t="s">
         <v>333</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="12" t="s">
         <v>315</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="20" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="16" t="s">
         <v>334</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="12" t="s">
         <v>316</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="20" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="16" t="s">
         <v>335</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="12" t="s">
         <v>327</v>
       </c>
-      <c r="D15" s="33" t="s">
+      <c r="D15" s="20" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="16" t="s">
         <v>336</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="12" t="s">
         <v>332</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D16" s="20" t="s">
         <v>378</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="16" t="s">
         <v>337</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="12" t="s">
         <v>314</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="20" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="16" t="s">
         <v>338</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="D18" s="30" t="s">
+      <c r="D18" s="17" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="16" t="s">
         <v>339</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="14" t="s">
         <v>288</v>
       </c>
-      <c r="D19" s="30" t="s">
+      <c r="D19" s="17" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="16" t="s">
         <v>340</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="14" t="s">
         <v>289</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="17" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="16" t="s">
         <v>341</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="14" t="s">
         <v>305</v>
       </c>
-      <c r="D21" s="30" t="s">
+      <c r="D21" s="17" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="16" t="s">
         <v>342</v>
       </c>
-      <c r="C22" s="27" t="s">
+      <c r="C22" s="14" t="s">
         <v>306</v>
       </c>
-      <c r="D22" s="30" t="s">
+      <c r="D22" s="17" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="16" t="s">
         <v>343</v>
       </c>
-      <c r="C23" s="27" t="s">
+      <c r="C23" s="14" t="s">
         <v>307</v>
       </c>
-      <c r="D23" s="30" t="s">
+      <c r="D23" s="17" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="16" t="s">
         <v>344</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="14" t="s">
         <v>308</v>
       </c>
-      <c r="D24" s="30" t="s">
+      <c r="D24" s="17" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="16" t="s">
         <v>345</v>
       </c>
-      <c r="C25" s="27" t="s">
+      <c r="C25" s="14" t="s">
         <v>309</v>
       </c>
-      <c r="D25" s="30" t="s">
+      <c r="D25" s="17" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="16" t="s">
         <v>346</v>
       </c>
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="14" t="s">
         <v>313</v>
       </c>
-      <c r="D26" s="30" t="s">
+      <c r="D26" s="17" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="16" t="s">
         <v>347</v>
       </c>
-      <c r="C27" s="27" t="s">
+      <c r="C27" s="14" t="s">
         <v>348</v>
       </c>
-      <c r="D27" s="30" t="s">
+      <c r="D27" s="17" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="16" t="s">
         <v>350</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="14" t="s">
         <v>351</v>
       </c>
-      <c r="D28" s="30" t="s">
+      <c r="D28" s="17" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="16" t="s">
         <v>360</v>
       </c>
-      <c r="C29" s="27" t="s">
+      <c r="C29" s="14" t="s">
         <v>364</v>
       </c>
-      <c r="D29" s="30" t="s">
+      <c r="D29" s="17" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="16" t="s">
         <v>367</v>
       </c>
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="14" t="s">
         <v>369</v>
       </c>
-      <c r="D30" s="30" t="s">
+      <c r="D30" s="17" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="34" t="s">
+      <c r="B31" s="21" t="s">
         <v>368</v>
       </c>
-      <c r="C31" s="35" t="s">
+      <c r="C31" s="22" t="s">
         <v>370</v>
       </c>
-      <c r="D31" s="36" t="s">
+      <c r="D31" s="23" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
-        <v>421</v>
+        <v>383</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>422</v>
+        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -3236,414 +3053,9 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="C3:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="3" width="54.140625" customWidth="1"/>
-    <col min="4" max="7" width="10.7109375" style="25" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="25" customWidth="1"/>
-    <col min="9" max="10" width="10.7109375" style="25" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="45" t="s">
-        <v>381</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="47"/>
-    </row>
-    <row r="2" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>382</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>383</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>417</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>384</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>385</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>387</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>388</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>389</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>391</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>392</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>394</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>394</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>394</v>
-      </c>
-      <c r="J3" s="18" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>396</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>397</v>
-      </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="J4" s="18" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>398</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>399</v>
-      </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="I5" s="17" t="s">
-        <v>400</v>
-      </c>
-      <c r="J5" s="18" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>401</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>402</v>
-      </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>395</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>400</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>395</v>
-      </c>
-      <c r="J6" s="18" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>403</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>404</v>
-      </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>400</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>400</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>395</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>395</v>
-      </c>
-      <c r="I7" s="17" t="s">
-        <v>395</v>
-      </c>
-      <c r="J7" s="18" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>405</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>406</v>
-      </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>400</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>400</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>394</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>394</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>395</v>
-      </c>
-      <c r="J8" s="18" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>407</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>408</v>
-      </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>400</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>395</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>395</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>395</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>395</v>
-      </c>
-      <c r="J9" s="18" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>409</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>410</v>
-      </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>400</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>395</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>395</v>
-      </c>
-      <c r="H10" s="17" t="s">
-        <v>395</v>
-      </c>
-      <c r="I10" s="17" t="s">
-        <v>395</v>
-      </c>
-      <c r="J10" s="18" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>411</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>412</v>
-      </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="I11" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="J11" s="18" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>413</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>414</v>
-      </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>400</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>395</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>395</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>395</v>
-      </c>
-      <c r="I12" s="17" t="s">
-        <v>395</v>
-      </c>
-      <c r="J12" s="18" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="21" t="s">
-        <v>415</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>418</v>
-      </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="23" t="s">
-        <v>393</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>400</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>416</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>395</v>
-      </c>
-      <c r="H13" s="23" t="s">
-        <v>395</v>
-      </c>
-      <c r="I13" s="23" t="s">
-        <v>395</v>
-      </c>
-      <c r="J13" s="24" t="s">
-        <v>395</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:D9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3:D9"/>
     </sheetView>
   </sheetViews>
@@ -3654,63 +3066,142 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="48" t="s">
-        <v>423</v>
-      </c>
-      <c r="D3" s="48" t="s">
-        <v>425</v>
+      <c r="C3" s="26" t="s">
+        <v>385</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="4" spans="3:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="C4" s="48" t="s">
-        <v>423</v>
-      </c>
-      <c r="D4" s="49" t="s">
-        <v>432</v>
+      <c r="C4" s="26" t="s">
+        <v>385</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="48" t="s">
-        <v>423</v>
-      </c>
-      <c r="D5" s="48" t="s">
-        <v>424</v>
+      <c r="C5" s="26" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="6" spans="3:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="C6" s="50" t="s">
-        <v>431</v>
-      </c>
-      <c r="D6" s="49" t="s">
-        <v>427</v>
+      <c r="C6" s="28" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="48" t="s">
-        <v>426</v>
-      </c>
-      <c r="D7" s="48" t="s">
-        <v>428</v>
+      <c r="C7" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="48" t="s">
-        <v>426</v>
-      </c>
-      <c r="D8" s="49" t="s">
-        <v>429</v>
+      <c r="C8" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="9" spans="3:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C9" s="48" t="s">
-        <v>426</v>
-      </c>
-      <c r="D9" s="49" t="s">
-        <v>430</v>
+      <c r="C9" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>392</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="11" t="s">
+        <v>404</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>402</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="12" t="s">
+        <v>396</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>395</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="12" t="s">
+        <v>396</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>398</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="12" t="s">
+        <v>396</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>400</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="12" t="s">
+        <v>396</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>401</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>397</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3773,7 +3264,7 @@
         <v>21</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>419</v>
+        <v>381</v>
       </c>
     </row>
     <row r="3" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
@@ -3903,7 +3394,7 @@
         <v>22</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>420</v>
+        <v>382</v>
       </c>
     </row>
     <row r="9" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
@@ -4473,7 +3964,7 @@
       <c r="E41" t="s">
         <v>227</v>
       </c>
-      <c r="F41" s="38" t="s">
+      <c r="F41" s="25" t="s">
         <v>189</v>
       </c>
       <c r="G41" t="s">
@@ -5326,10 +4817,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D22"/>
+  <dimension ref="B3:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5480,6 +4971,11 @@
       </c>
       <c r="C22" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
+        <v>399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated final report and action list
</commit_message>
<xml_diff>
--- a/Reports/Action List.xlsx
+++ b/Reports/Action List.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\WebProject\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="8" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="8" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Home Page" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Testing  Details '!$B$1:$H$57</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="407">
   <si>
     <t xml:space="preserve">lot of informaiton -  </t>
   </si>
@@ -934,44 +934,6 @@
 </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>You are Chatting With Option Box</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Provide details of chats you are having</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">People Who Like Me - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Displaying details of people who like my profile and may be interested in me</t>
-    </r>
-  </si>
-  <si>
     <t>Will display list of people who may be a match for me
 User needs to click on the photos that they want to do an action with</t>
   </si>
@@ -1023,36 +985,6 @@
 which will navigate them to screen to enter email and new password will be sent to email</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Possible Matches </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Photos allowing me the option to Like/Maybe/Goodbye/Report (see FN5)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">People Who  I Like </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Details of all the people I have liked and that I may find a match</t>
-    </r>
-  </si>
-  <si>
     <t>User can select photo of possible Match and Select the Like Button. This will  remove the Photo of this person from Possible Matches to People I have liked  View</t>
   </si>
   <si>
@@ -1077,15 +1009,9 @@
     <t>This section of the Meeting Space will provide me with Details of possible matches who liked my profile</t>
   </si>
   <si>
-    <t>User can select photo of person who liked my  Profile . Select the Like Button. If both users have liked each other this will automatically  initiate the chat line screen</t>
-  </si>
-  <si>
     <t>Chat Line</t>
   </si>
   <si>
-    <t>Meeting Space/Match Finder</t>
-  </si>
-  <si>
     <t>Meeting Space/Edit Profile</t>
   </si>
   <si>
@@ -1188,9 +1114,6 @@
     <t>Administrator Options</t>
   </si>
   <si>
-    <t xml:space="preserve">This option allows the Admin to manage the site.  </t>
-  </si>
-  <si>
     <t>FN5.101</t>
   </si>
   <si>
@@ -1263,603 +1186,13 @@
     <t>Same functionality as FNS3.104</t>
   </si>
   <si>
-    <r>
-      <t>H</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">eading Navigate Bar at the top </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">will display Name of the User and Allow them the option to Edit Profile,
-Edit Profile, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Remove their Profile from the Site, Logout of the Site</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Match Finder</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - this is a spontaneous function which allows the user look for matches under different criteria than stored in their Profile.   Facilitating the user if they are in a different location or indeed if they are looking for a different profile  at this moment.  This information is not stored in the Database </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Edit Profile</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> allows user to create a new profile or edit exiting profile. User is asked to enter  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>First Name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> , </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Surname</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> DOB</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Nearest City/Town</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Gender</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (allowing drop down option Male, Female, Transgender M-F or F-M ), </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Preferred Gender</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  (same validation per Gender)  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Seeking Min Age Profile</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (using slide bar ), </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Seeking Max Age Profile</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(using slide bar), </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Distance User will travel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (Using Distance bar)   </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Relationship type</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (Love,Casual,Friendship,Relatioship - Radio Buttons).  Validation limited due to drop down screens and radio buttons.  Mix /Max Age is validated.  Press </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Next</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> to take user to Second Profile details screen (Personal Details Page2  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>FN4.2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">)  or </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cancel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> which brings user back to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Meeting Space</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Edit Second Profile Page(Personal Details Page 2)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Allows the user to load their  Photograph, update some additional information in BIO box and select through radio buttons  Hobbies which are - Music, Sport, Travelling, Sailing, Food, Work,Family,Cooking,Gym  .  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>SAVE</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Remove Account</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> will navigate the user to screen which clearly calls out the implications of removing account - everything will be removed .  User is asked to Press </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Remove Account</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> if they want to continue to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cancel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (abort remove). If user selects Remove then ????? </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Adrian to advise what should happen as this aborts</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Logout</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Navigates user to Log Out Screen providing the user with option </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Logoff</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  or </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Cancel.
-Logoff  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>will bring user to screen to confirm they really want to logout which bring user back to logon screen</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.  Cancel </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>will bring user to</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Meeting Space</t>
-    </r>
-  </si>
-  <si>
     <t>This is a spontaneous option for the user to decide if they want to change some of their profile information to get meet a partner.  The user is presented with screen Gender Preference, Preferred location, Relationship type, Interests, Seeking Age.  All these  use the drop down screen which limits the user to the Mandatory Choices.</t>
   </si>
   <si>
-    <t>This screen is initiated from the meeting space screen.  User can send message to proposed match and start conversations and visa versa</t>
-  </si>
-  <si>
     <t>Adrian still working to perfection</t>
   </si>
   <si>
     <t>Deirdre to recheck</t>
-  </si>
-  <si>
-    <t>FN5.105</t>
   </si>
   <si>
     <t>Black list of words</t>
@@ -1929,6 +1262,729 @@
   </si>
   <si>
     <t>USER</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>You are Chatting With Option Box</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Provide details of chats you are having</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">People Who Like Me - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Displaying details of people who like my profile and may be interested in me</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">People Who  I Like </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Details of all the people I have liked and that I may find a match</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Edit Profile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> allows user to create a new profile or edit exiting profile. User is asked to enter  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>First Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> , </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Surname</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> DOB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nearest City/Town</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Gender</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (allowing drop down option Male, Female, Transgender M-F or F-M ), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Preferred Gender</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  (same validation per Gender)  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Seeking Min Age Profile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (using slide bar ), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Seeking Max Age Profile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(using slide bar), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Distance User will travel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Using Distance bar)   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Relationship type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Love,Casual,Friendship,Relatioship - Radio Buttons).  Validation limited due to drop down screens and radio buttons.  Mix /Max Age is validated.  Press </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Next</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to take user to Second Profile details screen (Personal Details Page2  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FN4.2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">)  or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cancel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> which brings user back to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Meeting Space</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Remove Account</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> will navigate the user to screen which clearly calls out the implications of removing account - everything will be removed .  User is asked to Press </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Remove Account</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> if they want to continue to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cancel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (abort remove). If user selects Remove then  account is  removed and user is brought back to logon screen.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Logout</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Navigates user to Log Out Screen providing the user with option </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Logoff</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Cancel.
+Logoff  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>will bring user to screen to confirm they really want to logout which bring user back to logon screen</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.  Cancel </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>will bring user to</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Meeting Space</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Heading Navigate Bar at the top </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">will display Name of the User and Allow them the option :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Edit Profile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Remove their Profile from the Site, Logout of the Site</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Match Finder</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - this is a spontaneous </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SEARCH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> function which allows the user look for matches under different criteria than stored in their Profile.   Facilitating the user if they are in a different location or indeed if they are looking for a different profile  at that moment.  This information is not stored in the Database </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Possible Matches </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Photos allowing the user the  option to Like/Maybe/Goodbye/Report (see FN5)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Edit Second Profile Page(Personal Details Page 2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Allows the user to load their  Photograph, update some additional information in BIO box and select through radio buttons  Hobbies which are - Music, Sport, Travelling, Sailing, Food, Work,Family,Cooking,Gym  .  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">SAVE
+Please note Phot is not saved on profile until date is SAVED. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>User can validate this by  viewing Profile after update</t>
+    </r>
+  </si>
+  <si>
+    <t>Meeting Space/Match Finder
+(SEARCH FUNCTIONALITY)</t>
+  </si>
+  <si>
+    <t>User can select photo of person who liked their Profile . Select the Like Button. If both users have liked each other this will automatically  initiate the option to chat screen</t>
+  </si>
+  <si>
+    <t>This option allows the Admin to manage the site.  
+User has to log on with Specific Logon and Password (Details outlined in Useful Password Section )
+Once user successful logs in they will be pesented with Admin screen and a phot of users who have been reported  by other users or who haeve been automatically reporting due to the use of bad language</t>
+  </si>
+  <si>
+    <t>Blacklist words can only be maintained using SQL statements by the DBA</t>
+  </si>
+  <si>
+    <t>This screen is initiated from the meeting space screen.  User can send message to proposed match and start conversations and visa versa.
+Chat begins - the system will automatically check  conversation and dentifies the use of black listed words and reports this to the Systadmin  if the word is used more than 5 times.
+It also takes the liberty of  blocking communication being seen by the other user</t>
+  </si>
+  <si>
+    <t>Click Photo to view why this person was reported.
+If there is evidence of an offence the Sysadmin can suspend the user for 1 month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   FN5.105</t>
   </si>
 </sst>
 </file>
@@ -1979,21 +2035,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2010,6 +2051,21 @@
     <font>
       <sz val="16"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2258,9 +2314,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -2284,52 +2340,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2340,23 +2360,68 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2699,6 +2764,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2706,339 +2772,342 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="110.5703125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="27" customWidth="1"/>
+    <col min="3" max="3" width="70.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="111.85546875" style="25" customWidth="1"/>
     <col min="5" max="5" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
-        <v>371</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>372</v>
-      </c>
-      <c r="D3" s="13" t="s">
+    <row r="3" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B3" s="12" t="s">
+        <v>364</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>365</v>
+      </c>
+      <c r="D3" s="24" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="24" t="s">
+    <row r="4" spans="2:5" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="B4" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="18" t="s">
         <v>280</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="19" t="s">
         <v>276</v>
       </c>
       <c r="E4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="16" t="s">
+    <row r="5" spans="2:5" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="B5" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="18" t="s">
         <v>269</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
+      <c r="D5" s="19" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="93" x14ac:dyDescent="0.35">
+      <c r="B6" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="18" t="s">
         <v>281</v>
       </c>
-      <c r="D6" s="17" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="32" t="s">
+      <c r="D6" s="19" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="35" t="s">
         <v>279</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="20" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="33"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="17" t="s">
-        <v>374</v>
+    <row r="8" spans="2:5" ht="196.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="36"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="19" t="s">
+        <v>397</v>
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="33"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="17" t="s">
-        <v>284</v>
+    <row r="9" spans="2:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="36"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="19" t="s">
+        <v>391</v>
       </c>
       <c r="E9" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="33"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="19" t="s">
-        <v>302</v>
+    <row r="10" spans="2:5" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="B10" s="36"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="21" t="s">
+        <v>398</v>
       </c>
       <c r="E10" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="33"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="19" t="s">
-        <v>285</v>
+    <row r="11" spans="2:5" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="B11" s="36"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="21" t="s">
+        <v>392</v>
       </c>
       <c r="E11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="34"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="19" t="s">
-        <v>303</v>
+    <row r="12" spans="2:5" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="B12" s="37"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="21" t="s">
+        <v>393</v>
       </c>
       <c r="E12" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="B13" s="16" t="s">
+    <row r="13" spans="2:5" ht="232.5" x14ac:dyDescent="0.35">
+      <c r="B13" s="17" t="s">
+        <v>327</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="139.5" x14ac:dyDescent="0.35">
+      <c r="B14" s="17" t="s">
+        <v>328</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="116.25" x14ac:dyDescent="0.35">
+      <c r="B15" s="17" t="s">
+        <v>329</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>321</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="93" x14ac:dyDescent="0.35">
+      <c r="B16" s="17" t="s">
+        <v>330</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>326</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="116.25" x14ac:dyDescent="0.35">
+      <c r="B17" s="17" t="s">
+        <v>331</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>400</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="17" t="s">
+        <v>332</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="B19" s="17" t="s">
         <v>333</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B14" s="16" t="s">
+      <c r="C19" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="B20" s="17" t="s">
         <v>334</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B15" s="16" t="s">
+      <c r="C20" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="93" x14ac:dyDescent="0.35">
+      <c r="B21" s="17" t="s">
         <v>335</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>327</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B16" s="16" t="s">
+      <c r="C21" s="18" t="s">
+        <v>301</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="B22" s="17" t="s">
         <v>336</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>332</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B17" s="16" t="s">
+      <c r="C22" s="18" t="s">
+        <v>302</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="B23" s="17" t="s">
         <v>337</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>314</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="16" t="s">
+      <c r="C23" s="18" t="s">
+        <v>303</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="B24" s="17" t="s">
         <v>338</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>287</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="16" t="s">
+      <c r="C24" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="B25" s="17" t="s">
         <v>339</v>
       </c>
-      <c r="C19" s="14" t="s">
-        <v>288</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="16" t="s">
+      <c r="C25" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="162.75" x14ac:dyDescent="0.35">
+      <c r="B26" s="17" t="s">
         <v>340</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>289</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B21" s="16" t="s">
+      <c r="C26" s="18" t="s">
+        <v>308</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="139.5" x14ac:dyDescent="0.35">
+      <c r="B27" s="17" t="s">
         <v>341</v>
       </c>
-      <c r="C21" s="14" t="s">
-        <v>305</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="16" t="s">
+      <c r="C27" s="18" t="s">
         <v>342</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>306</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="16" t="s">
+      <c r="D27" s="19" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B28" s="17" t="s">
         <v>343</v>
       </c>
-      <c r="C23" s="14" t="s">
-        <v>307</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="16" t="s">
+      <c r="C28" s="18" t="s">
         <v>344</v>
       </c>
-      <c r="C24" s="14" t="s">
-        <v>308</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="16" t="s">
-        <v>345</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>309</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="16" t="s">
-        <v>346</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>313</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="16" t="s">
-        <v>347</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>348</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="16" t="s">
-        <v>350</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>351</v>
-      </c>
-      <c r="D28" s="17" t="s">
+      <c r="D28" s="19" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="B29" s="17" t="s">
+        <v>353</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B30" s="17" t="s">
+        <v>360</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>362</v>
+      </c>
+      <c r="D30" s="19" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="16" t="s">
-        <v>360</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>364</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="16" t="s">
-        <v>367</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>369</v>
-      </c>
-      <c r="D30" s="17" t="s">
+    <row r="31" spans="2:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B31" s="31" t="s">
+        <v>361</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>363</v>
+      </c>
+      <c r="D31" s="23" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="31" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="21" t="s">
-        <v>368</v>
-      </c>
-      <c r="C31" s="22" t="s">
+    <row r="32" spans="2:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="26" t="s">
+        <v>406</v>
+      </c>
+      <c r="C32" s="30" t="s">
         <v>370</v>
       </c>
-      <c r="D31" s="23" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="6" t="s">
-        <v>383</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>384</v>
+      <c r="D32" s="23" t="s">
+        <v>403</v>
       </c>
     </row>
   </sheetData>
@@ -3066,63 +3135,64 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="26" t="s">
-        <v>385</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>387</v>
+      <c r="C3" s="14" t="s">
+        <v>371</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="4" spans="3:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="C4" s="26" t="s">
-        <v>385</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>394</v>
+      <c r="C4" s="14" t="s">
+        <v>371</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="26" t="s">
-        <v>385</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>386</v>
+      <c r="C5" s="14" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="6" spans="3:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="C6" s="28" t="s">
-        <v>393</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>389</v>
+      <c r="C6" s="16" t="s">
+        <v>379</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="26" t="s">
-        <v>388</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>390</v>
+      <c r="C7" s="14" t="s">
+        <v>374</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="26" t="s">
-        <v>388</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>391</v>
+      <c r="C8" s="14" t="s">
+        <v>374</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="9" spans="3:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C9" s="26" t="s">
-        <v>388</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>392</v>
+      <c r="C9" s="14" t="s">
+        <v>374</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>378</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3130,7 +3200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3:E7"/>
     </sheetView>
   </sheetViews>
@@ -3142,58 +3212,58 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C3" s="11" t="s">
-        <v>404</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>402</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>403</v>
+      <c r="C3" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C4" s="12" t="s">
-        <v>396</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>395</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>397</v>
+      <c r="C4" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="12" t="s">
-        <v>396</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>398</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>397</v>
+      <c r="C5" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>384</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="12" t="s">
-        <v>396</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>400</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>397</v>
+      <c r="C6" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="12" t="s">
-        <v>396</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>401</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>397</v>
+      <c r="C7" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>387</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>383</v>
       </c>
     </row>
   </sheetData>
@@ -3264,7 +3334,7 @@
         <v>21</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
     </row>
     <row r="3" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
@@ -3394,7 +3464,7 @@
         <v>22</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
     </row>
     <row r="9" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
@@ -3964,7 +4034,7 @@
       <c r="E41" t="s">
         <v>227</v>
       </c>
-      <c r="F41" s="25" t="s">
+      <c r="F41" s="13" t="s">
         <v>189</v>
       </c>
       <c r="G41" t="s">
@@ -4102,13 +4172,13 @@
     </row>
     <row r="48" spans="2:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
+        <v>290</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="F48" s="3" t="s">
         <v>292</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>293</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>294</v>
       </c>
       <c r="G48" t="s">
         <v>6</v>
@@ -4116,19 +4186,19 @@
     </row>
     <row r="49" spans="2:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
+        <v>294</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>296</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>298</v>
       </c>
       <c r="E49" t="s">
         <v>239</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G49" t="s">
         <v>8</v>
@@ -4136,64 +4206,64 @@
     </row>
     <row r="50" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="G50" t="s">
         <v>59</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
     </row>
     <row r="51" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="G51" t="s">
         <v>21</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="52" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="G52" t="s">
         <v>21</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="53" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="G53" t="s">
         <v>21</v>
@@ -4201,13 +4271,13 @@
     </row>
     <row r="54" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="G54" t="s">
         <v>21</v>
@@ -4215,13 +4285,13 @@
     </row>
     <row r="55" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="G55" t="s">
         <v>21</v>
@@ -4229,13 +4299,13 @@
     </row>
     <row r="56" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="C56" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="D56" s="3" t="s">
         <v>358</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>365</v>
       </c>
       <c r="G56" t="s">
         <v>21</v>
@@ -4243,13 +4313,13 @@
     </row>
     <row r="57" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="G57" t="s">
         <v>21</v>
@@ -4329,6 +4399,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4413,6 +4484,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4670,6 +4742,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4684,6 +4757,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4975,7 +5049,7 @@
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>399</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
action list and doc again
</commit_message>
<xml_diff>
--- a/Reports/Action List.xlsx
+++ b/Reports/Action List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="8" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Home Page" sheetId="2" r:id="rId1"/>
@@ -26,9 +26,9 @@
     <sheet name="logon&amp;passwords" sheetId="19" r:id="rId12"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Testing  Details '!$B$1:$H$57</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Testing  Details '!$B$1:$H$63</definedName>
   </definedNames>
-  <calcPr calcId="171027" refMode="R1C1"/>
+  <calcPr calcId="152511" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="423">
   <si>
     <t xml:space="preserve">lot of informaiton -  </t>
   </si>
@@ -1024,18 +1024,12 @@
     <t>Save button on profile page 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Not working </t>
-  </si>
-  <si>
     <t>Test50</t>
   </si>
   <si>
     <t>Cancel Button on Profile Page 1</t>
   </si>
   <si>
-    <t>Aborting</t>
-  </si>
-  <si>
     <t>Send email to all</t>
   </si>
   <si>
@@ -1057,9 +1051,6 @@
     <t xml:space="preserve">return button after removal </t>
   </si>
   <si>
-    <t>ABorting</t>
-  </si>
-  <si>
     <t>I removed Deirdre1.Shanahn1 and all went well untik final screen to return and it aborts.  Thinking this should take you back to logon screen</t>
   </si>
   <si>
@@ -1159,9 +1150,6 @@
     <t>Administrator  Options -Suspend 1 Month</t>
   </si>
   <si>
-    <t>takes to view profile . I don’t know if we have time but Admin should not display the options to like /etc</t>
-  </si>
-  <si>
     <t>Removes the option for the person to join out app ever again</t>
   </si>
   <si>
@@ -1187,9 +1175,6 @@
   </si>
   <si>
     <t>This is a spontaneous option for the user to decide if they want to change some of their profile information to get meet a partner.  The user is presented with screen Gender Preference, Preferred location, Relationship type, Interests, Seeking Age.  All these  use the drop down screen which limits the user to the Mandatory Choices.</t>
-  </si>
-  <si>
-    <t>Adrian still working to perfection</t>
   </si>
   <si>
     <t>Deirdre to recheck</t>
@@ -1985,6 +1970,73 @@
   </si>
   <si>
     <t xml:space="preserve">   FN5.105</t>
+  </si>
+  <si>
+    <t>Test67</t>
+  </si>
+  <si>
+    <t>new user</t>
+  </si>
+  <si>
+    <t>test68</t>
+  </si>
+  <si>
+    <t>Match Finder</t>
+  </si>
+  <si>
+    <t>true/false</t>
+  </si>
+  <si>
+    <t>test69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meeting space  </t>
+  </si>
+  <si>
+    <t>selected someone in you are chatting with box. Press view, then in View press like</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aborted with errr  </t>
+  </si>
+  <si>
+    <t>Allows me to select NO interests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test 70 </t>
+  </si>
+  <si>
+    <t>email sent to Adrian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Searched everything on match finder
+</t>
+  </si>
+  <si>
+    <t>2 issues
+ lisa sharp there multiple times (maybe she has multiple emails)
+same issues as before  Like Like (Duplicated)</t>
+  </si>
+  <si>
+    <t>Test71</t>
+  </si>
+  <si>
+    <t>Aborted</t>
+  </si>
+  <si>
+    <t>takes to view profile . I don’t know if we have time but Admin should not display the options to like /etc
+you should have an option to go back</t>
+  </si>
+  <si>
+    <t>when I  view a match  and then like it bring me to chat when it should be in people  who I like box</t>
+  </si>
+  <si>
+    <t>OPEN</t>
+  </si>
+  <si>
+    <t>Told this is fine</t>
+  </si>
+  <si>
+    <t>Suspend but I don’t know if suspended</t>
   </si>
 </sst>
 </file>
@@ -2772,7 +2824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -2786,10 +2838,10 @@
   <sheetData>
     <row r="3" spans="2:5" ht="21" x14ac:dyDescent="0.35">
       <c r="B3" s="12" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D3" s="24" t="s">
         <v>223</v>
@@ -2846,7 +2898,7 @@
       <c r="B8" s="36"/>
       <c r="C8" s="33"/>
       <c r="D8" s="19" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="E8" s="3"/>
     </row>
@@ -2854,7 +2906,7 @@
       <c r="B9" s="36"/>
       <c r="C9" s="33"/>
       <c r="D9" s="19" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="E9" t="s">
         <v>101</v>
@@ -2864,7 +2916,7 @@
       <c r="B10" s="36"/>
       <c r="C10" s="33"/>
       <c r="D10" s="21" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="E10" t="s">
         <v>101</v>
@@ -2874,7 +2926,7 @@
       <c r="B11" s="36"/>
       <c r="C11" s="33"/>
       <c r="D11" s="21" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="E11" t="s">
         <v>101</v>
@@ -2884,7 +2936,7 @@
       <c r="B12" s="37"/>
       <c r="C12" s="34"/>
       <c r="D12" s="21" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="E12" t="s">
         <v>101</v>
@@ -2892,62 +2944,62 @@
     </row>
     <row r="13" spans="2:5" ht="232.5" x14ac:dyDescent="0.35">
       <c r="B13" s="17" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>309</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="139.5" x14ac:dyDescent="0.35">
       <c r="B14" s="17" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C14" s="18" t="s">
         <v>310</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="116.25" x14ac:dyDescent="0.35">
       <c r="B15" s="17" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="93" x14ac:dyDescent="0.35">
       <c r="B16" s="17" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="116.25" x14ac:dyDescent="0.35">
       <c r="B17" s="17" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="17" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C18" s="18" t="s">
         <v>285</v>
@@ -2958,7 +3010,7 @@
     </row>
     <row r="19" spans="2:4" ht="69.75" x14ac:dyDescent="0.35">
       <c r="B19" s="17" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>286</v>
@@ -2969,7 +3021,7 @@
     </row>
     <row r="20" spans="2:4" ht="69.75" x14ac:dyDescent="0.35">
       <c r="B20" s="17" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C20" s="18" t="s">
         <v>287</v>
@@ -2980,7 +3032,7 @@
     </row>
     <row r="21" spans="2:4" ht="93" x14ac:dyDescent="0.35">
       <c r="B21" s="17" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>301</v>
@@ -2991,7 +3043,7 @@
     </row>
     <row r="22" spans="2:4" ht="69.75" x14ac:dyDescent="0.35">
       <c r="B22" s="17" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C22" s="18" t="s">
         <v>302</v>
@@ -3002,7 +3054,7 @@
     </row>
     <row r="23" spans="2:4" ht="69.75" x14ac:dyDescent="0.35">
       <c r="B23" s="17" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>303</v>
@@ -3013,7 +3065,7 @@
     </row>
     <row r="24" spans="2:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="B24" s="17" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C24" s="18" t="s">
         <v>304</v>
@@ -3024,90 +3076,90 @@
     </row>
     <row r="25" spans="2:4" ht="69.75" x14ac:dyDescent="0.35">
       <c r="B25" s="17" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>305</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="162.75" x14ac:dyDescent="0.35">
       <c r="B26" s="17" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C26" s="18" t="s">
         <v>308</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="139.5" x14ac:dyDescent="0.35">
       <c r="B27" s="17" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
     </row>
     <row r="28" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B28" s="17" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="69.75" x14ac:dyDescent="0.35">
       <c r="B29" s="17" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B30" s="17" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B31" s="31" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B32" s="26" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -3136,58 +3188,58 @@
   <sheetData>
     <row r="3" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C3" s="14" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
     </row>
     <row r="4" spans="3:4" ht="45" x14ac:dyDescent="0.25">
       <c r="C4" s="14" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C5" s="14" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
     </row>
     <row r="6" spans="3:4" ht="60" x14ac:dyDescent="0.25">
       <c r="C6" s="16" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C7" s="14" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C8" s="14" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
     </row>
     <row r="9" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C9" s="14" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
     </row>
   </sheetData>
@@ -3213,57 +3265,57 @@
   <sheetData>
     <row r="3" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C3" s="10" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C4" s="11" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C5" s="11" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C6" s="11" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C7" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>382</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>387</v>
-      </c>
       <c r="E7" s="11" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
   </sheetData>
@@ -3278,11 +3330,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="B1:H57"/>
+  <dimension ref="B1:H63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3314,7 +3366,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>110</v>
       </c>
@@ -3331,10 +3383,10 @@
         <v>107</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>368</v>
+        <v>421</v>
       </c>
     </row>
     <row r="3" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
@@ -3464,7 +3516,7 @@
         <v>22</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
     </row>
     <row r="9" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
@@ -3754,7 +3806,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>180</v>
       </c>
@@ -3766,6 +3818,9 @@
       </c>
       <c r="E23" t="s">
         <v>240</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>422</v>
       </c>
       <c r="G23" t="s">
         <v>21</v>
@@ -4212,100 +4267,103 @@
         <v>312</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>313</v>
+        <v>6</v>
       </c>
       <c r="G50" t="s">
         <v>59</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="51" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
+        <v>313</v>
+      </c>
+      <c r="C51" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="D51" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G51" t="s">
+        <v>21</v>
+      </c>
+      <c r="H51" s="3" t="s">
         <v>315</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="G51" t="s">
-        <v>21</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="52" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="G52" t="s">
         <v>21</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="53" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
+        <v>320</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="F53" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="C53" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>325</v>
-      </c>
       <c r="G53" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="G54" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
+        <v>345</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="G55" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>347</v>
+      </c>
+      <c r="C56" s="7" t="s">
         <v>348</v>
       </c>
-      <c r="C55" s="7" t="s">
-        <v>346</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="G55" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="56" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>350</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>351</v>
-      </c>
       <c r="D56" s="3" t="s">
-        <v>358</v>
+        <v>418</v>
       </c>
       <c r="G56" t="s">
         <v>21</v>
@@ -4313,23 +4371,101 @@
     </row>
     <row r="57" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="G57" t="s">
         <v>21</v>
       </c>
     </row>
+    <row r="58" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>402</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="G58" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>404</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="G59" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>407</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="G60" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>412</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D63" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:H57">
+  <autoFilter ref="B1:H63">
     <filterColumn colId="5">
       <filters>
-        <filter val="Open"/>
+        <filter val="open"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -5049,7 +5185,7 @@
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated FN4.105 action list
</commit_message>
<xml_diff>
--- a/Reports/Action List.xlsx
+++ b/Reports/Action List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Home Page" sheetId="2" r:id="rId1"/>
@@ -2116,10 +2116,6 @@
 (SEARCH/BROWSE  FUNCTIONALITY)</t>
   </si>
   <si>
-    <t>Will display list of people who may be a match for me
-User needs to click on the photos that they want to do an action</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">User can select photo of possible Match and Select the Like Button. This will  remove the Photo of this person from </t>
     </r>
@@ -2338,6 +2334,24 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Will display list of people who may be a match for me
+User needs to click on the photos that they want to do an action
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please note we have provided the user the ability to see all possible matches even those who do not match their preferred Gender</t>
     </r>
   </si>
 </sst>
@@ -2789,6 +2803,9 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2806,9 +2823,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3159,8 +3173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E34"/>
   <sheetViews>
-    <sheetView topLeftCell="B28" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3219,10 +3233,10 @@
       </c>
     </row>
     <row r="7" spans="2:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="38" t="s">
         <v>278</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="35" t="s">
         <v>142</v>
       </c>
       <c r="D7" s="20" t="s">
@@ -3230,16 +3244,16 @@
       </c>
     </row>
     <row r="8" spans="2:5" ht="196.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="38"/>
-      <c r="C8" s="35"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="36"/>
       <c r="D8" s="19" t="s">
         <v>408</v>
       </c>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="2:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="38"/>
-      <c r="C9" s="35"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="19" t="s">
         <v>374</v>
       </c>
@@ -3248,8 +3262,8 @@
       </c>
     </row>
     <row r="10" spans="2:5" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="B10" s="38"/>
-      <c r="C10" s="35"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="21" t="s">
         <v>379</v>
       </c>
@@ -3258,8 +3272,8 @@
       </c>
     </row>
     <row r="11" spans="2:5" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="B11" s="38"/>
-      <c r="C11" s="35"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="36"/>
       <c r="D11" s="21" t="s">
         <v>375</v>
       </c>
@@ -3268,8 +3282,8 @@
       </c>
     </row>
     <row r="12" spans="2:5" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="B12" s="39"/>
-      <c r="C12" s="36"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="37"/>
       <c r="D12" s="21" t="s">
         <v>376</v>
       </c>
@@ -3332,7 +3346,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="17" t="s">
         <v>319</v>
       </c>
@@ -3340,7 +3354,7 @@
         <v>283</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>413</v>
+        <v>428</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="69.75" x14ac:dyDescent="0.35">
@@ -3351,7 +3365,7 @@
         <v>284</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="69.75" x14ac:dyDescent="0.35">
@@ -3362,7 +3376,7 @@
         <v>285</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="93" x14ac:dyDescent="0.35">
@@ -3373,7 +3387,7 @@
         <v>294</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="69.75" x14ac:dyDescent="0.35">
@@ -3395,7 +3409,7 @@
         <v>296</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="46.5" x14ac:dyDescent="0.35">
@@ -3406,7 +3420,7 @@
         <v>297</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="93" x14ac:dyDescent="0.35">
@@ -3417,7 +3431,7 @@
         <v>298</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="162.75" x14ac:dyDescent="0.35">
@@ -3428,7 +3442,7 @@
         <v>299</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="162.75" x14ac:dyDescent="0.35">
@@ -3439,7 +3453,7 @@
         <v>329</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="28" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
@@ -3483,7 +3497,7 @@
         <v>349</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.4">
@@ -3494,29 +3508,29 @@
         <v>407</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B33" s="26" t="s">
         <v>405</v>
       </c>
-      <c r="C33" s="40" t="s">
-        <v>423</v>
+      <c r="C33" s="34" t="s">
+        <v>422</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B34" s="26" t="s">
+        <v>423</v>
+      </c>
+      <c r="C34" s="29" t="s">
+        <v>425</v>
+      </c>
+      <c r="D34" s="23" t="s">
         <v>424</v>
-      </c>
-      <c r="C34" s="29" t="s">
-        <v>426</v>
-      </c>
-      <c r="D34" s="23" t="s">
-        <v>425</v>
       </c>
     </row>
   </sheetData>
@@ -5555,7 +5569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>